<commit_message>
New Assets and vision for Output of resource collection
Output of resource collection (page 12) (vision doc)
new food items
new resources
</commit_message>
<xml_diff>
--- a/Game Design/Assets.xlsx
+++ b/Game Design/Assets.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="105" windowWidth="15120" windowHeight="8010"/>
+    <workbookView xWindow="120" yWindow="105" windowWidth="15120" windowHeight="8010" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Weapons" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'Food Items'!$A$1:$T$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Magic!$A$1:$W$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Opponents!$A$1:$AD$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Resources!$A$1:$O$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Resources!$A$1:$S$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Weapons!$A$1:$T$4</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="639" uniqueCount="228">
   <si>
     <t>Name</t>
   </si>
@@ -315,15 +315,9 @@
     <t>Mountains</t>
   </si>
   <si>
-    <t>Icy planes</t>
-  </si>
-  <si>
     <t>Swamps</t>
   </si>
   <si>
-    <t>Prairie/Savannah</t>
-  </si>
-  <si>
     <t>Forest?</t>
   </si>
   <si>
@@ -643,13 +637,91 @@
   </si>
   <si>
     <t>Resistance</t>
+  </si>
+  <si>
+    <t>Ice</t>
+  </si>
+  <si>
+    <t>Def. Quantity</t>
+  </si>
+  <si>
+    <t>Collect Quantity</t>
+  </si>
+  <si>
+    <t>Apple</t>
+  </si>
+  <si>
+    <t>Potatoe</t>
+  </si>
+  <si>
+    <t>?planting</t>
+  </si>
+  <si>
+    <t>Green Herb</t>
+  </si>
+  <si>
+    <t>Purple Flower</t>
+  </si>
+  <si>
+    <t>Herb</t>
+  </si>
+  <si>
+    <t>Green Tea</t>
+  </si>
+  <si>
+    <t>Potions 1</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>2 Green Herb</t>
+  </si>
+  <si>
+    <t>Green Soup</t>
+  </si>
+  <si>
+    <t>3 Pea</t>
+  </si>
+  <si>
+    <t>1 Root</t>
+  </si>
+  <si>
+    <t>Purple Ale</t>
+  </si>
+  <si>
+    <t>3 Purple Flower</t>
+  </si>
+  <si>
+    <t>4 Barries</t>
+  </si>
+  <si>
+    <t>Barry Juice</t>
+  </si>
+  <si>
+    <t>Strong Ale</t>
+  </si>
+  <si>
+    <t>Potions 2</t>
+  </si>
+  <si>
+    <t>Grassland</t>
+  </si>
+  <si>
+    <t>Dry</t>
+  </si>
+  <si>
+    <t>Moderate</t>
+  </si>
+  <si>
+    <t>Wet</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="8">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1169,19 +1241,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="1" fillId="2" borderId="9" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
@@ -1190,6 +1250,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="9" fontId="1" fillId="2" borderId="9" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Ausgabe" xfId="5" builtinId="21"/>
@@ -1207,11 +1279,16 @@
       <color rgb="FFF7F5DF"/>
     </mruColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa-Design">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
   <a:themeElements>
     <a:clrScheme name="Larissa">
       <a:dk1>
@@ -1285,6 +1362,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1319,6 +1397,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Larissa">
@@ -1494,14 +1573,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16:N16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.7109375" customWidth="1"/>
     <col min="2" max="2" width="13.28515625" customWidth="1"/>
@@ -1523,15 +1602,15 @@
     <col min="20" max="20" width="11.42578125" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="15.75" thickBot="1">
+    <row r="1" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="26" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C1" s="26" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>1</v>
@@ -1543,7 +1622,7 @@
         <v>3</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>4</v>
@@ -1585,12 +1664,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:20">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>53</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D2" s="9" t="s">
         <v>29</v>
@@ -1626,12 +1705,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:20">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>54</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D3" s="9" t="s">
         <v>29</v>
@@ -1667,12 +1746,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:20">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>55</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D4" s="9" t="s">
         <v>29</v>
@@ -1708,12 +1787,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:20">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>56</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D5" s="9" t="s">
         <v>29</v>
@@ -1749,12 +1828,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:20">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>60</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D6" s="9" t="s">
         <v>18</v>
@@ -1781,12 +1860,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:20">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>17</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D7" s="9" t="s">
         <v>18</v>
@@ -1822,12 +1901,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:20">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>23</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D8" s="9" t="s">
         <v>18</v>
@@ -1869,12 +1948,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:20">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>26</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D9" s="9" t="s">
         <v>18</v>
@@ -1907,12 +1986,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:20">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>28</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D10" s="9" t="s">
         <v>29</v>
@@ -1951,12 +2030,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:20">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>31</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D11" s="9" t="s">
         <v>29</v>
@@ -2001,12 +2080,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:20">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>33</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D12" s="9" t="s">
         <v>29</v>
@@ -2048,12 +2127,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:20">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>34</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D13" s="9" t="s">
         <v>29</v>
@@ -2083,12 +2162,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:20">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>41</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D14" s="9" t="s">
         <v>29</v>
@@ -2118,12 +2197,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:20">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>43</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D15" s="9" t="s">
         <v>29</v>
@@ -2153,12 +2232,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:20">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>51</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D16" s="9" t="s">
         <v>52</v>
@@ -2191,12 +2270,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:20">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>58</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D17" s="9" t="s">
         <v>52</v>
@@ -2223,12 +2302,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:20">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>36</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D18" s="9" t="s">
         <v>29</v>
@@ -2264,12 +2343,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:20">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>38</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D19" s="9" t="s">
         <v>29</v>
@@ -2305,12 +2384,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:20">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>45</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D20" s="9" t="s">
         <v>29</v>
@@ -2340,12 +2419,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:20">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>46</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D21" s="9" t="s">
         <v>47</v>
@@ -2378,12 +2457,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:20">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>48</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D22" s="9" t="s">
         <v>47</v>
@@ -2416,12 +2495,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:20">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>61</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D23" s="9" t="s">
         <v>47</v>
@@ -2430,12 +2509,12 @@
         <v>49</v>
       </c>
     </row>
-    <row r="24" spans="1:20">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>62</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D24" s="9" t="s">
         <v>29</v>
@@ -2444,221 +2523,221 @@
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="1:20">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>63</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="M25" s="9" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="26" spans="1:20">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>64</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="M26" s="9" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="27" spans="1:20">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>65</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="M27" s="9" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="28" spans="1:20">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>66</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="M28" s="9" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="29" spans="1:20">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>68</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="M29" s="9" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="30" spans="1:20">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>69</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="M30" s="9" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="31" spans="1:20">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>70</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="M31" s="9" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="32" spans="1:20">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>72</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="M32" s="9" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="33" spans="1:13">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>73</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="M33" s="9" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="34" spans="1:13">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>74</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="M34" s="9" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="35" spans="1:13">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>75</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="M35" s="9" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="36" spans="1:13">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>76</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="M36" s="9" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="37" spans="1:13">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>78</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="M37" s="9" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="38" spans="1:13">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>79</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="M38" s="9" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="39" spans="1:13">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>80</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="M39" s="9" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="40" spans="1:13">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>81</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="M40" s="9" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="41" spans="1:13">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>83</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="M41" s="9" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="42" spans="1:13">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>84</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="M42" s="9" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="43" spans="1:13">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>85</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="M43" s="9" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="44" spans="1:13">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>86</v>
       </c>
       <c r="C44" s="9" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="M44" s="9" t="s">
         <v>82</v>
@@ -2666,8 +2745,6 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:T4">
-    <filterColumn colId="1"/>
-    <filterColumn colId="2"/>
     <sortState ref="A2:T44">
       <sortCondition ref="G1:G4"/>
     </sortState>
@@ -2678,42 +2755,42 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J2" sqref="J2:K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.28515625" customWidth="1"/>
     <col min="2" max="18" width="11.42578125" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="32" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C1" s="32" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D1" s="28" t="s">
         <v>1</v>
@@ -2722,13 +2799,13 @@
         <v>2</v>
       </c>
       <c r="F1" s="28" t="s">
+        <v>143</v>
+      </c>
+      <c r="G1" s="28" t="s">
+        <v>144</v>
+      </c>
+      <c r="H1" s="28" t="s">
         <v>145</v>
-      </c>
-      <c r="G1" s="28" t="s">
-        <v>146</v>
-      </c>
-      <c r="H1" s="28" t="s">
-        <v>147</v>
       </c>
       <c r="I1" s="28" t="s">
         <v>8</v>
@@ -2758,21 +2835,21 @@
         <v>16</v>
       </c>
       <c r="R1" s="33" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>137</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="E2" s="24" t="s">
         <v>139</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>138</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>140</v>
-      </c>
-      <c r="E2" s="24" t="s">
-        <v>141</v>
       </c>
       <c r="F2" s="9">
         <v>2</v>
@@ -2784,7 +2861,7 @@
         <v>21</v>
       </c>
       <c r="K2" s="9" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="L2" s="9">
         <v>1</v>
@@ -2793,15 +2870,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E3" s="23" t="s">
         <v>27</v>
@@ -2816,7 +2893,7 @@
         <v>21</v>
       </c>
       <c r="K3" s="9" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="L3" s="9">
         <v>1</v>
@@ -2825,18 +2902,18 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E4" s="24" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F4" s="9">
         <v>0</v>
@@ -2848,7 +2925,7 @@
         <v>21</v>
       </c>
       <c r="K4" s="9" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="L4" s="9">
         <v>1</v>
@@ -2865,27 +2942,27 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="20" customFormat="1">
+    <row r="1" spans="1:23" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="27" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C1" s="27" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D1" s="28" t="s">
         <v>1</v>
@@ -2894,28 +2971,28 @@
         <v>2</v>
       </c>
       <c r="F1" s="28" t="s">
+        <v>149</v>
+      </c>
+      <c r="G1" s="28" t="s">
+        <v>144</v>
+      </c>
+      <c r="H1" s="28" t="s">
+        <v>150</v>
+      </c>
+      <c r="I1" s="28" t="s">
         <v>151</v>
       </c>
-      <c r="G1" s="28" t="s">
-        <v>146</v>
-      </c>
-      <c r="H1" s="28" t="s">
+      <c r="J1" s="28" t="s">
         <v>152</v>
       </c>
-      <c r="I1" s="28" t="s">
-        <v>153</v>
-      </c>
-      <c r="J1" s="28" t="s">
-        <v>154</v>
-      </c>
       <c r="K1" s="28" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="L1" s="28" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="M1" s="28" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="N1" s="28" t="s">
         <v>4</v>
@@ -2948,16 +3025,16 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:23">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B2" s="9"/>
       <c r="C2" s="9" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E2" s="22" t="s">
         <v>19</v>
@@ -2978,7 +3055,7 @@
         <v>21</v>
       </c>
       <c r="Q2" s="9" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="R2" s="9">
         <v>2</v>
@@ -2992,29 +3069,21 @@
       <c r="W2" s="9"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:W1">
-    <filterColumn colId="6"/>
-    <filterColumn colId="7"/>
-    <filterColumn colId="8"/>
-    <filterColumn colId="9"/>
-    <filterColumn colId="10"/>
-    <filterColumn colId="11"/>
-    <filterColumn colId="12"/>
-  </autoFilter>
+  <autoFilter ref="A1:W1"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P7" sqref="P7"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="11.42578125" style="9"/>
     <col min="4" max="11" width="11.42578125" style="9"/>
@@ -3025,106 +3094,106 @@
     <col min="18" max="28" width="11.42578125" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" s="20" customFormat="1">
+    <row r="1" spans="1:30" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="32" t="s">
+        <v>155</v>
+      </c>
+      <c r="C1" s="32" t="s">
+        <v>135</v>
+      </c>
+      <c r="D1" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="28" t="s">
+        <v>156</v>
+      </c>
+      <c r="F1" s="28" t="s">
         <v>157</v>
       </c>
-      <c r="C1" s="32" t="s">
-        <v>137</v>
-      </c>
-      <c r="D1" s="32" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="28" t="s">
+      <c r="G1" s="28" t="s">
         <v>158</v>
       </c>
-      <c r="F1" s="28" t="s">
+      <c r="H1" s="28" t="s">
         <v>159</v>
       </c>
-      <c r="G1" s="28" t="s">
+      <c r="I1" s="28" t="s">
         <v>160</v>
       </c>
-      <c r="H1" s="28" t="s">
+      <c r="J1" s="28" t="s">
         <v>161</v>
-      </c>
-      <c r="I1" s="28" t="s">
-        <v>162</v>
-      </c>
-      <c r="J1" s="28" t="s">
-        <v>163</v>
       </c>
       <c r="K1" s="28" t="s">
         <v>7</v>
       </c>
       <c r="L1" s="28" t="s">
+        <v>170</v>
+      </c>
+      <c r="M1" s="28" t="s">
+        <v>171</v>
+      </c>
+      <c r="N1" s="28" t="s">
+        <v>162</v>
+      </c>
+      <c r="O1" s="28" t="s">
+        <v>163</v>
+      </c>
+      <c r="P1" s="28" t="s">
+        <v>201</v>
+      </c>
+      <c r="Q1" s="28" t="s">
+        <v>164</v>
+      </c>
+      <c r="R1" s="34" t="s">
         <v>172</v>
       </c>
-      <c r="M1" s="28" t="s">
+      <c r="S1" s="34" t="s">
         <v>173</v>
       </c>
-      <c r="N1" s="28" t="s">
-        <v>164</v>
-      </c>
-      <c r="O1" s="28" t="s">
+      <c r="T1" s="36" t="s">
+        <v>182</v>
+      </c>
+      <c r="U1" s="36" t="s">
+        <v>179</v>
+      </c>
+      <c r="V1" s="36" t="s">
+        <v>180</v>
+      </c>
+      <c r="W1" s="36" t="s">
+        <v>181</v>
+      </c>
+      <c r="X1" s="30" t="s">
         <v>165</v>
       </c>
-      <c r="P1" s="28" t="s">
-        <v>203</v>
-      </c>
-      <c r="Q1" s="28" t="s">
+      <c r="Y1" s="30" t="s">
         <v>166</v>
       </c>
-      <c r="R1" s="34" t="s">
-        <v>174</v>
-      </c>
-      <c r="S1" s="34" t="s">
-        <v>175</v>
-      </c>
-      <c r="T1" s="36" t="s">
-        <v>184</v>
-      </c>
-      <c r="U1" s="36" t="s">
-        <v>181</v>
-      </c>
-      <c r="V1" s="36" t="s">
-        <v>182</v>
-      </c>
-      <c r="W1" s="36" t="s">
-        <v>183</v>
-      </c>
-      <c r="X1" s="30" t="s">
+      <c r="Z1" s="30" t="s">
         <v>167</v>
       </c>
-      <c r="Y1" s="30" t="s">
+      <c r="AA1" s="30" t="s">
         <v>168</v>
       </c>
-      <c r="Z1" s="30" t="s">
+      <c r="AB1" s="30" t="s">
         <v>169</v>
-      </c>
-      <c r="AA1" s="30" t="s">
-        <v>170</v>
-      </c>
-      <c r="AB1" s="30" t="s">
-        <v>171</v>
       </c>
       <c r="AC1" s="30"/>
       <c r="AD1" s="21"/>
     </row>
-    <row r="2" spans="1:30">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>175</v>
+      </c>
+      <c r="B2" s="9">
+        <v>1</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="D2" s="9" t="s">
         <v>177</v>
-      </c>
-      <c r="B2" s="9">
-        <v>1</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>138</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>179</v>
       </c>
       <c r="E2" s="9">
         <v>3</v>
@@ -3161,13 +3230,13 @@
       </c>
       <c r="P2" s="37"/>
       <c r="Q2" s="9" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="R2" s="9" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="S2" s="9" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="T2" s="9">
         <v>1</v>
@@ -3188,18 +3257,18 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:30">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>174</v>
+      </c>
+      <c r="B3" s="9">
+        <v>1</v>
+      </c>
+      <c r="C3" s="35" t="s">
         <v>176</v>
       </c>
-      <c r="B3" s="9">
-        <v>1</v>
-      </c>
-      <c r="C3" s="35" t="s">
-        <v>178</v>
-      </c>
       <c r="D3" s="9" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E3" s="9">
         <v>9</v>
@@ -3236,13 +3305,13 @@
       </c>
       <c r="P3" s="37"/>
       <c r="Q3" s="9" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="R3" s="9" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="S3" s="9" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="T3" s="9">
         <v>2</v>
@@ -3254,7 +3323,7 @@
         <v>1</v>
       </c>
       <c r="W3" s="9" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="X3" s="37" t="s">
         <v>52</v>
@@ -3264,1314 +3333,1695 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AD1">
-    <filterColumn colId="10"/>
-    <filterColumn colId="15"/>
-    <filterColumn colId="18"/>
-    <filterColumn colId="19"/>
-    <filterColumn colId="20"/>
-    <filterColumn colId="21"/>
-    <filterColumn colId="22"/>
-  </autoFilter>
+  <autoFilter ref="A1:AD1"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O36"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="34.85546875" customWidth="1"/>
     <col min="2" max="2" width="11.42578125" style="9"/>
     <col min="4" max="4" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.85546875" customWidth="1"/>
-    <col min="7" max="7" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.7109375" customWidth="1"/>
-    <col min="14" max="14" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="62.28515625" customWidth="1"/>
+    <col min="5" max="5" width="8.85546875" customWidth="1"/>
+    <col min="6" max="6" width="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875" customWidth="1"/>
+    <col min="8" max="8" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.42578125" customWidth="1"/>
+    <col min="11" max="11" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.7109375" customWidth="1"/>
+    <col min="16" max="16" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.7109375" customWidth="1"/>
+    <col min="18" max="18" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="62.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15.75" thickBot="1">
+    <row r="1" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="14" t="s">
         <v>87</v>
       </c>
       <c r="B1" s="32" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C1" s="32" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D1" s="15" t="s">
         <v>88</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
       <c r="F1" s="15" t="s">
+        <v>199</v>
+      </c>
+      <c r="G1" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="G1" s="15" t="s">
+      <c r="H1" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="I1" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="I1" s="17" t="s">
+      <c r="J1" s="16" t="s">
+        <v>204</v>
+      </c>
+      <c r="K1" s="16" t="s">
+        <v>203</v>
+      </c>
+      <c r="L1" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="J1" s="18" t="s">
+      <c r="M1" s="18" t="s">
         <v>93</v>
       </c>
-      <c r="K1" s="18" t="s">
+      <c r="N1" s="18" t="s">
+        <v>202</v>
+      </c>
+      <c r="O1" s="18" t="s">
+        <v>169</v>
+      </c>
+      <c r="P1" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="L1" s="18" t="s">
+      <c r="Q1" s="18" t="s">
+        <v>224</v>
+      </c>
+      <c r="R1" s="18" t="s">
         <v>95</v>
       </c>
-      <c r="M1" s="18" t="s">
+      <c r="S1" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="N1" s="18" t="s">
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="O1" s="19" t="s">
+      <c r="B2" s="21">
+        <v>1</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="D2" s="21" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="2" spans="1:15">
-      <c r="A2" s="20" t="s">
+      <c r="E2" s="21"/>
+      <c r="F2" s="21">
+        <v>1</v>
+      </c>
+      <c r="G2" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="H2" s="21"/>
+      <c r="I2" s="21">
+        <v>4</v>
+      </c>
+      <c r="J2" s="21">
+        <v>3</v>
+      </c>
+      <c r="K2" s="21">
+        <v>3</v>
+      </c>
+      <c r="L2" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="M2" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="N2" s="21"/>
+      <c r="O2" s="21"/>
+      <c r="P2" s="21"/>
+      <c r="Q2" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="R2" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="S2" s="21"/>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" s="20" t="s">
         <v>99</v>
       </c>
-      <c r="B2" s="21">
-        <v>1</v>
-      </c>
-      <c r="C2" s="21" t="s">
-        <v>138</v>
-      </c>
-      <c r="D2" s="21" t="s">
+      <c r="B3" s="21">
+        <v>1</v>
+      </c>
+      <c r="C3" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="D3" s="21" t="s">
+        <v>98</v>
+      </c>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21">
+        <v>1</v>
+      </c>
+      <c r="G3" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21">
+        <v>6</v>
+      </c>
+      <c r="J3" s="21">
+        <v>3</v>
+      </c>
+      <c r="K3" s="21">
+        <v>3</v>
+      </c>
+      <c r="L3" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="M3" s="21"/>
+      <c r="N3" s="21"/>
+      <c r="O3" s="21"/>
+      <c r="P3" s="21"/>
+      <c r="Q3" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="R3" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="S3" s="21"/>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="B4" s="21">
+        <v>2</v>
+      </c>
+      <c r="C4" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="D4" s="21" t="s">
+        <v>98</v>
+      </c>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21">
+        <v>1</v>
+      </c>
+      <c r="G4" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="H4" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="I4" s="21">
+        <v>6</v>
+      </c>
+      <c r="J4" s="21">
+        <v>3</v>
+      </c>
+      <c r="K4" s="21">
+        <v>3</v>
+      </c>
+      <c r="L4" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="M4" s="21"/>
+      <c r="N4" s="21"/>
+      <c r="O4" s="21"/>
+      <c r="P4" s="21"/>
+      <c r="Q4" s="21"/>
+      <c r="R4" s="21"/>
+      <c r="S4" s="21"/>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="B5" s="21">
+        <v>2</v>
+      </c>
+      <c r="C5" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="D5" s="21" t="s">
+        <v>98</v>
+      </c>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21">
+        <v>1</v>
+      </c>
+      <c r="G5" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="H5" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="I5" s="21">
+        <v>8</v>
+      </c>
+      <c r="J5" s="21">
+        <v>3</v>
+      </c>
+      <c r="K5" s="21">
+        <v>6</v>
+      </c>
+      <c r="L5" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="M5" s="21"/>
+      <c r="N5" s="21"/>
+      <c r="O5" s="21"/>
+      <c r="P5" s="21"/>
+      <c r="Q5" s="21"/>
+      <c r="R5" s="21"/>
+      <c r="S5" s="21"/>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6" s="20" t="s">
         <v>100</v>
       </c>
-      <c r="E2" s="21">
-        <v>1</v>
-      </c>
-      <c r="F2" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
-      <c r="I2" s="21" t="s">
+      <c r="B6" s="21">
+        <v>2</v>
+      </c>
+      <c r="C6" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="D6" s="21" t="s">
+        <v>98</v>
+      </c>
+      <c r="E6" s="21"/>
+      <c r="F6" s="21">
+        <v>2</v>
+      </c>
+      <c r="G6" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="H6" s="21"/>
+      <c r="I6" s="21">
+        <v>8</v>
+      </c>
+      <c r="J6" s="21">
+        <v>2</v>
+      </c>
+      <c r="K6" s="21">
+        <v>2</v>
+      </c>
+      <c r="L6" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="J2" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="K2" s="21"/>
-      <c r="L2" s="21"/>
-      <c r="M2" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="N2" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="O2" s="21"/>
-    </row>
-    <row r="3" spans="1:15">
-      <c r="A3" s="20" t="s">
-        <v>101</v>
-      </c>
-      <c r="B3" s="21">
-        <v>1</v>
-      </c>
-      <c r="C3" s="21" t="s">
-        <v>138</v>
-      </c>
-      <c r="D3" s="21" t="s">
-        <v>100</v>
-      </c>
-      <c r="E3" s="21">
-        <v>1</v>
-      </c>
-      <c r="F3" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="G3" s="21"/>
-      <c r="H3" s="21"/>
-      <c r="I3" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="J3" s="21"/>
-      <c r="K3" s="21"/>
-      <c r="L3" s="21"/>
-      <c r="M3" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="N3" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="O3" s="21"/>
-    </row>
-    <row r="4" spans="1:15">
-      <c r="A4" s="20" t="s">
-        <v>102</v>
-      </c>
-      <c r="B4" s="21"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="21" t="s">
-        <v>100</v>
-      </c>
-      <c r="E4" s="21">
-        <v>2</v>
-      </c>
-      <c r="F4" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="G4" s="21"/>
-      <c r="H4" s="21"/>
-      <c r="I4" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="J4" s="21"/>
-      <c r="K4" s="21"/>
-      <c r="L4" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="M4" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="N4" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="O4" s="21"/>
-    </row>
-    <row r="5" spans="1:15">
-      <c r="A5" s="20" t="s">
-        <v>103</v>
-      </c>
-      <c r="B5" s="21"/>
-      <c r="C5" s="20"/>
-      <c r="D5" s="21" t="s">
-        <v>104</v>
-      </c>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="G5" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="H5" s="21"/>
-      <c r="I5" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="J5" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="K5" s="21"/>
-      <c r="L5" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="M5" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="N5" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="O5" s="21"/>
-    </row>
-    <row r="6" spans="1:15">
-      <c r="A6" s="20" t="s">
-        <v>187</v>
-      </c>
-      <c r="B6" s="21"/>
-      <c r="C6" s="20"/>
-      <c r="D6" s="21" t="s">
-        <v>104</v>
-      </c>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="G6" s="21"/>
-      <c r="H6" s="21"/>
-      <c r="I6" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="J6" s="21"/>
-      <c r="K6" s="21"/>
-      <c r="L6" s="21"/>
       <c r="M6" s="21"/>
       <c r="N6" s="21"/>
       <c r="O6" s="21"/>
-    </row>
-    <row r="7" spans="1:15">
+      <c r="P6" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q6" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="R6" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="S6" s="21"/>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
-        <v>105</v>
+        <v>125</v>
       </c>
       <c r="B7" s="21"/>
       <c r="C7" s="20"/>
       <c r="D7" s="21" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="E7" s="21"/>
-      <c r="F7" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="G7" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="H7" s="21"/>
-      <c r="I7" s="21" t="s">
-        <v>21</v>
-      </c>
+      <c r="F7" s="21"/>
+      <c r="G7" s="21"/>
+      <c r="H7" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="I7" s="21"/>
       <c r="J7" s="21"/>
       <c r="K7" s="21"/>
-      <c r="L7" s="21"/>
+      <c r="L7" s="21" t="s">
+        <v>67</v>
+      </c>
       <c r="M7" s="21"/>
       <c r="N7" s="21"/>
       <c r="O7" s="21"/>
-    </row>
-    <row r="8" spans="1:15">
+      <c r="P7" s="21"/>
+      <c r="Q7" s="21"/>
+      <c r="R7" s="21"/>
+      <c r="S7" s="21"/>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
-        <v>106</v>
+        <v>126</v>
       </c>
       <c r="B8" s="21"/>
       <c r="C8" s="20"/>
       <c r="D8" s="21" t="s">
-        <v>100</v>
-      </c>
-      <c r="E8" s="21">
-        <v>2</v>
-      </c>
-      <c r="F8" s="21" t="s">
-        <v>52</v>
-      </c>
+        <v>98</v>
+      </c>
+      <c r="E8" s="21"/>
+      <c r="F8" s="21"/>
       <c r="G8" s="21"/>
-      <c r="H8" s="21"/>
-      <c r="I8" s="21" t="s">
-        <v>49</v>
-      </c>
+      <c r="H8" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="I8" s="21"/>
       <c r="J8" s="21"/>
       <c r="K8" s="21"/>
-      <c r="L8" s="21"/>
+      <c r="L8" s="21" t="s">
+        <v>67</v>
+      </c>
       <c r="M8" s="21"/>
       <c r="N8" s="21"/>
       <c r="O8" s="21"/>
-    </row>
-    <row r="9" spans="1:15">
+      <c r="P8" s="21"/>
+      <c r="Q8" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="R8" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="S8" s="21"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
-        <v>107</v>
+        <v>124</v>
       </c>
       <c r="B9" s="21"/>
       <c r="C9" s="20"/>
       <c r="D9" s="21" t="s">
-        <v>100</v>
-      </c>
-      <c r="E9" s="21">
-        <v>2</v>
-      </c>
-      <c r="F9" s="21" t="s">
-        <v>52</v>
-      </c>
+        <v>98</v>
+      </c>
+      <c r="E9" s="21"/>
+      <c r="F9" s="21"/>
       <c r="G9" s="21"/>
-      <c r="H9" s="21"/>
-      <c r="I9" s="21" t="s">
-        <v>49</v>
-      </c>
+      <c r="H9" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="I9" s="21"/>
       <c r="J9" s="21"/>
       <c r="K9" s="21"/>
-      <c r="L9" s="21"/>
+      <c r="L9" s="21" t="s">
+        <v>67</v>
+      </c>
       <c r="M9" s="21"/>
       <c r="N9" s="21"/>
       <c r="O9" s="21"/>
-    </row>
-    <row r="10" spans="1:15">
+      <c r="P9" s="21"/>
+      <c r="Q9" s="21"/>
+      <c r="R9" s="21"/>
+      <c r="S9" s="21"/>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
-        <v>108</v>
+        <v>130</v>
       </c>
       <c r="B10" s="21"/>
       <c r="C10" s="20"/>
       <c r="D10" s="21" t="s">
-        <v>100</v>
-      </c>
-      <c r="E10" s="21">
-        <v>1</v>
-      </c>
-      <c r="F10" s="21" t="s">
-        <v>52</v>
-      </c>
+        <v>98</v>
+      </c>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
       <c r="G10" s="21" t="s">
         <v>52</v>
       </c>
       <c r="H10" s="21"/>
-      <c r="I10" s="21" t="s">
-        <v>49</v>
-      </c>
+      <c r="I10" s="21"/>
       <c r="J10" s="21"/>
       <c r="K10" s="21"/>
-      <c r="L10" s="21"/>
+      <c r="L10" s="21" t="s">
+        <v>21</v>
+      </c>
       <c r="M10" s="21"/>
       <c r="N10" s="21"/>
       <c r="O10" s="21"/>
-    </row>
-    <row r="11" spans="1:15">
+      <c r="P10" s="21"/>
+      <c r="Q10" s="21"/>
+      <c r="R10" s="21"/>
+      <c r="S10" s="21"/>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
-        <v>109</v>
+        <v>131</v>
       </c>
       <c r="B11" s="21"/>
       <c r="C11" s="20"/>
       <c r="D11" s="21" t="s">
-        <v>100</v>
-      </c>
-      <c r="E11" s="21">
-        <v>1</v>
-      </c>
-      <c r="F11" s="21" t="s">
-        <v>52</v>
-      </c>
+        <v>98</v>
+      </c>
+      <c r="E11" s="21"/>
+      <c r="F11" s="21"/>
       <c r="G11" s="21" t="s">
         <v>52</v>
       </c>
       <c r="H11" s="21"/>
-      <c r="I11" s="21" t="s">
-        <v>49</v>
-      </c>
+      <c r="I11" s="21"/>
       <c r="J11" s="21"/>
       <c r="K11" s="21"/>
-      <c r="L11" s="21"/>
+      <c r="L11" s="21" t="s">
+        <v>21</v>
+      </c>
       <c r="M11" s="21"/>
       <c r="N11" s="21"/>
       <c r="O11" s="21"/>
-    </row>
-    <row r="12" spans="1:15">
+      <c r="P11" s="21"/>
+      <c r="Q11" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="R11" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="S11" s="21"/>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
-        <v>110</v>
+        <v>132</v>
       </c>
       <c r="B12" s="21"/>
       <c r="C12" s="20"/>
       <c r="D12" s="21" t="s">
-        <v>100</v>
-      </c>
-      <c r="E12" s="21">
-        <v>3</v>
-      </c>
+        <v>98</v>
+      </c>
+      <c r="E12" s="21"/>
       <c r="F12" s="21"/>
       <c r="G12" s="21" t="s">
         <v>52</v>
       </c>
       <c r="H12" s="21"/>
-      <c r="I12" s="21" t="s">
-        <v>67</v>
-      </c>
+      <c r="I12" s="21"/>
       <c r="J12" s="21"/>
       <c r="K12" s="21"/>
-      <c r="L12" s="21"/>
+      <c r="L12" s="21" t="s">
+        <v>21</v>
+      </c>
       <c r="M12" s="21"/>
       <c r="N12" s="21"/>
       <c r="O12" s="21"/>
-    </row>
-    <row r="13" spans="1:15">
-      <c r="A13" s="20" t="s">
-        <v>111</v>
-      </c>
+      <c r="P12" s="21"/>
+      <c r="Q12" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="R12" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="S12" s="21"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A13" s="20"/>
       <c r="B13" s="21"/>
       <c r="C13" s="20"/>
-      <c r="D13" s="21" t="s">
-        <v>100</v>
-      </c>
+      <c r="D13" s="21"/>
       <c r="E13" s="21"/>
       <c r="F13" s="21"/>
-      <c r="G13" s="21" t="s">
-        <v>52</v>
-      </c>
+      <c r="G13" s="21"/>
       <c r="H13" s="21"/>
-      <c r="I13" s="21" t="s">
-        <v>67</v>
-      </c>
+      <c r="I13" s="21"/>
       <c r="J13" s="21"/>
       <c r="K13" s="21"/>
       <c r="L13" s="21"/>
       <c r="M13" s="21"/>
       <c r="N13" s="21"/>
       <c r="O13" s="21"/>
-    </row>
-    <row r="14" spans="1:15">
+      <c r="P13" s="21"/>
+      <c r="Q13" s="21"/>
+      <c r="R13" s="21"/>
+      <c r="S13" s="21"/>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="20" t="s">
-        <v>112</v>
-      </c>
-      <c r="B14" s="21"/>
-      <c r="C14" s="20"/>
+        <v>205</v>
+      </c>
+      <c r="B14" s="21">
+        <v>1</v>
+      </c>
+      <c r="C14" s="21" t="s">
+        <v>136</v>
+      </c>
       <c r="D14" s="21" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E14" s="21"/>
-      <c r="F14" s="21"/>
+      <c r="F14" s="21">
+        <v>1</v>
+      </c>
       <c r="G14" s="21" t="s">
         <v>52</v>
       </c>
       <c r="H14" s="21"/>
-      <c r="I14" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="J14" s="21"/>
-      <c r="K14" s="21"/>
-      <c r="L14" s="21"/>
+      <c r="I14" s="21">
+        <v>5</v>
+      </c>
+      <c r="J14" s="21">
+        <v>4</v>
+      </c>
+      <c r="K14" s="21">
+        <v>4</v>
+      </c>
+      <c r="L14" s="21" t="s">
+        <v>21</v>
+      </c>
       <c r="M14" s="21"/>
       <c r="N14" s="21"/>
       <c r="O14" s="21"/>
-    </row>
-    <row r="15" spans="1:15">
+      <c r="P14" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q14" s="21"/>
+      <c r="R14" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="S14" s="21"/>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="20" t="s">
-        <v>113</v>
-      </c>
-      <c r="B15" s="21"/>
-      <c r="C15" s="20"/>
+        <v>206</v>
+      </c>
+      <c r="B15" s="21">
+        <v>1</v>
+      </c>
+      <c r="C15" s="21" t="s">
+        <v>136</v>
+      </c>
       <c r="D15" s="21" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E15" s="21"/>
-      <c r="F15" s="21"/>
+      <c r="F15" s="21">
+        <v>2</v>
+      </c>
       <c r="G15" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="H15" s="21"/>
-      <c r="I15" s="21" t="s">
+      <c r="H15" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="I15" s="21">
+        <v>6</v>
+      </c>
+      <c r="J15" s="21">
+        <v>3</v>
+      </c>
+      <c r="K15" s="21">
+        <v>3</v>
+      </c>
+      <c r="L15" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="J15" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="K15" s="21"/>
-      <c r="L15" s="21"/>
       <c r="M15" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="N15" s="21" t="s">
-        <v>52</v>
-      </c>
+      <c r="N15" s="21"/>
       <c r="O15" s="21"/>
-    </row>
-    <row r="16" spans="1:15">
-      <c r="A16" s="20" t="s">
-        <v>114</v>
-      </c>
+      <c r="P15" s="21"/>
+      <c r="Q15" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="R15" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="S15" s="21"/>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A16" s="20"/>
       <c r="B16" s="21"/>
       <c r="C16" s="20"/>
-      <c r="D16" s="21" t="s">
-        <v>100</v>
-      </c>
+      <c r="D16" s="21"/>
       <c r="E16" s="21"/>
       <c r="F16" s="21"/>
-      <c r="G16" s="21" t="s">
-        <v>52</v>
-      </c>
+      <c r="G16" s="21"/>
       <c r="H16" s="21"/>
-      <c r="I16" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="J16" s="21" t="s">
-        <v>52</v>
-      </c>
+      <c r="I16" s="21"/>
+      <c r="J16" s="21"/>
       <c r="K16" s="21"/>
       <c r="L16" s="21"/>
-      <c r="M16" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="N16" s="21" t="s">
-        <v>52</v>
-      </c>
+      <c r="M16" s="21"/>
+      <c r="N16" s="21"/>
       <c r="O16" s="21"/>
-    </row>
-    <row r="17" spans="1:15">
+      <c r="P16" s="21"/>
+      <c r="Q16" s="21"/>
+      <c r="R16" s="21"/>
+      <c r="S16" s="21"/>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
-        <v>115</v>
-      </c>
-      <c r="B17" s="21"/>
-      <c r="C17" s="20"/>
+        <v>208</v>
+      </c>
+      <c r="B17" s="21">
+        <v>1</v>
+      </c>
+      <c r="C17" s="21" t="s">
+        <v>136</v>
+      </c>
       <c r="D17" s="21" t="s">
-        <v>104</v>
+        <v>210</v>
       </c>
       <c r="E17" s="21"/>
-      <c r="F17" s="21"/>
+      <c r="F17" s="21">
+        <v>0</v>
+      </c>
       <c r="G17" s="21" t="s">
         <v>52</v>
       </c>
       <c r="H17" s="21"/>
-      <c r="I17" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="J17" s="21"/>
-      <c r="K17" s="21"/>
-      <c r="L17" s="21"/>
+      <c r="I17" s="21">
+        <v>5</v>
+      </c>
+      <c r="J17" s="21">
+        <v>1</v>
+      </c>
+      <c r="K17" s="21">
+        <v>2</v>
+      </c>
+      <c r="L17" s="21" t="s">
+        <v>49</v>
+      </c>
       <c r="M17" s="21"/>
       <c r="N17" s="21"/>
       <c r="O17" s="21"/>
-    </row>
-    <row r="18" spans="1:15">
+      <c r="P17" s="21"/>
+      <c r="Q17" s="21"/>
+      <c r="R17" s="21"/>
+      <c r="S17" s="21"/>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="20" t="s">
-        <v>202</v>
-      </c>
-      <c r="B18" s="21"/>
-      <c r="C18" s="20"/>
+        <v>209</v>
+      </c>
+      <c r="B18" s="21">
+        <v>2</v>
+      </c>
+      <c r="C18" s="21" t="s">
+        <v>136</v>
+      </c>
       <c r="D18" s="21" t="s">
-        <v>116</v>
-      </c>
-      <c r="E18" s="21">
-        <v>3</v>
-      </c>
-      <c r="F18" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="G18" s="21"/>
+        <v>210</v>
+      </c>
+      <c r="E18" s="21"/>
+      <c r="F18" s="21">
+        <v>0</v>
+      </c>
+      <c r="G18" s="21" t="s">
+        <v>52</v>
+      </c>
       <c r="H18" s="21"/>
-      <c r="I18" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="J18" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="K18" s="21" t="s">
-        <v>52</v>
+      <c r="I18" s="21">
+        <v>6</v>
+      </c>
+      <c r="J18" s="21">
+        <v>2</v>
+      </c>
+      <c r="K18" s="21">
+        <v>2</v>
       </c>
       <c r="L18" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="M18" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="N18" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="O18" s="21" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15">
-      <c r="A19" s="20" t="s">
-        <v>118</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="M18" s="21"/>
+      <c r="N18" s="21"/>
+      <c r="O18" s="21"/>
+      <c r="P18" s="21"/>
+      <c r="Q18" s="21"/>
+      <c r="R18" s="21"/>
+      <c r="S18" s="21"/>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A19" s="20"/>
       <c r="B19" s="21"/>
       <c r="C19" s="20"/>
-      <c r="D19" s="21" t="s">
-        <v>104</v>
-      </c>
+      <c r="D19" s="21"/>
       <c r="E19" s="21"/>
-      <c r="F19" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="G19" s="21" t="s">
-        <v>52</v>
-      </c>
+      <c r="F19" s="21"/>
+      <c r="G19" s="21"/>
       <c r="H19" s="21"/>
-      <c r="I19" s="21" t="s">
-        <v>119</v>
-      </c>
+      <c r="I19" s="21"/>
       <c r="J19" s="21"/>
       <c r="K19" s="21"/>
       <c r="L19" s="21"/>
       <c r="M19" s="21"/>
       <c r="N19" s="21"/>
-      <c r="O19" s="21" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15">
+      <c r="O19" s="21"/>
+      <c r="P19" s="21"/>
+      <c r="Q19" s="21"/>
+      <c r="R19" s="21"/>
+      <c r="S19" s="21"/>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" s="20" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="B20" s="21"/>
       <c r="C20" s="20"/>
       <c r="D20" s="21" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="E20" s="21"/>
-      <c r="F20" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="G20" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="H20" s="21"/>
-      <c r="I20" s="21" t="s">
-        <v>122</v>
-      </c>
+      <c r="F20" s="21"/>
+      <c r="G20" s="21"/>
+      <c r="H20" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="I20" s="21"/>
       <c r="J20" s="21"/>
       <c r="K20" s="21"/>
-      <c r="L20" s="21"/>
-      <c r="M20" s="21"/>
+      <c r="L20" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="M20" s="21" t="s">
+        <v>52</v>
+      </c>
       <c r="N20" s="21"/>
-      <c r="O20" s="21" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15">
+      <c r="O20" s="21"/>
+      <c r="P20" s="21"/>
+      <c r="Q20" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="R20" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="S20" s="21" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" s="20" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="B21" s="21"/>
       <c r="C21" s="20"/>
       <c r="D21" s="21" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="E21" s="21"/>
-      <c r="F21" s="21" t="s">
-        <v>52</v>
-      </c>
+      <c r="F21" s="21"/>
       <c r="G21" s="21" t="s">
         <v>52</v>
       </c>
       <c r="H21" s="21"/>
-      <c r="I21" s="21" t="s">
-        <v>124</v>
-      </c>
+      <c r="I21" s="21"/>
       <c r="J21" s="21"/>
       <c r="K21" s="21"/>
-      <c r="L21" s="21"/>
+      <c r="L21" s="21" t="s">
+        <v>21</v>
+      </c>
       <c r="M21" s="21"/>
       <c r="N21" s="21"/>
-      <c r="O21" s="21" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15">
+      <c r="O21" s="21"/>
+      <c r="P21" s="21"/>
+      <c r="Q21" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="R21" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="S21" s="21"/>
+    </row>
+    <row r="22" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="20" t="s">
-        <v>125</v>
+        <v>104</v>
       </c>
       <c r="B22" s="21"/>
       <c r="C22" s="20"/>
       <c r="D22" s="21" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="E22" s="21"/>
-      <c r="F22" s="21" t="s">
-        <v>52</v>
+      <c r="F22" s="21">
+        <v>2</v>
       </c>
       <c r="G22" s="21" t="s">
         <v>52</v>
       </c>
       <c r="H22" s="21"/>
-      <c r="I22" s="21" t="s">
-        <v>21</v>
-      </c>
+      <c r="I22" s="21"/>
       <c r="J22" s="21"/>
       <c r="K22" s="21"/>
-      <c r="L22" s="21"/>
+      <c r="L22" s="21" t="s">
+        <v>49</v>
+      </c>
       <c r="M22" s="21"/>
       <c r="N22" s="21"/>
       <c r="O22" s="21"/>
-    </row>
-    <row r="23" spans="1:15">
+      <c r="P22" s="21"/>
+      <c r="Q22" s="21"/>
+      <c r="R22" s="21"/>
+      <c r="S22" s="21"/>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" s="20" t="s">
-        <v>126</v>
+        <v>105</v>
       </c>
       <c r="B23" s="21"/>
       <c r="C23" s="20"/>
       <c r="D23" s="21" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E23" s="21"/>
-      <c r="F23" s="21"/>
+      <c r="F23" s="21">
+        <v>2</v>
+      </c>
       <c r="G23" s="21" t="s">
         <v>52</v>
       </c>
       <c r="H23" s="21"/>
-      <c r="I23" s="21" t="s">
-        <v>67</v>
-      </c>
+      <c r="I23" s="21"/>
       <c r="J23" s="21"/>
       <c r="K23" s="21"/>
-      <c r="L23" s="21"/>
+      <c r="L23" s="21" t="s">
+        <v>49</v>
+      </c>
       <c r="M23" s="21"/>
       <c r="N23" s="21"/>
       <c r="O23" s="21"/>
-    </row>
-    <row r="24" spans="1:15">
+      <c r="P23" s="21"/>
+      <c r="Q23" s="21"/>
+      <c r="R23" s="21"/>
+      <c r="S23" s="21"/>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" s="20" t="s">
-        <v>127</v>
+        <v>108</v>
       </c>
       <c r="B24" s="21"/>
       <c r="C24" s="20"/>
       <c r="D24" s="21" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E24" s="21"/>
-      <c r="F24" s="21"/>
-      <c r="G24" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="H24" s="21"/>
-      <c r="I24" s="21" t="s">
-        <v>67</v>
-      </c>
+      <c r="F24" s="21">
+        <v>3</v>
+      </c>
+      <c r="G24" s="21"/>
+      <c r="H24" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="I24" s="21"/>
       <c r="J24" s="21"/>
       <c r="K24" s="21"/>
-      <c r="L24" s="21"/>
+      <c r="L24" s="21" t="s">
+        <v>67</v>
+      </c>
       <c r="M24" s="21"/>
       <c r="N24" s="21"/>
       <c r="O24" s="21"/>
-    </row>
-    <row r="25" spans="1:15">
+      <c r="P24" s="21"/>
+      <c r="Q24" s="21"/>
+      <c r="R24" s="21"/>
+      <c r="S24" s="21"/>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" s="20" t="s">
-        <v>128</v>
+        <v>109</v>
       </c>
       <c r="B25" s="21"/>
       <c r="C25" s="20"/>
       <c r="D25" s="21" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E25" s="21"/>
       <c r="F25" s="21"/>
-      <c r="G25" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="H25" s="21"/>
-      <c r="I25" s="21" t="s">
-        <v>67</v>
-      </c>
+      <c r="G25" s="21"/>
+      <c r="H25" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="I25" s="21"/>
       <c r="J25" s="21"/>
       <c r="K25" s="21"/>
-      <c r="L25" s="21"/>
-      <c r="M25" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="N25" s="21" t="s">
-        <v>52</v>
-      </c>
+      <c r="L25" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="M25" s="21"/>
+      <c r="N25" s="21"/>
       <c r="O25" s="21"/>
-    </row>
-    <row r="26" spans="1:15">
+      <c r="P25" s="21"/>
+      <c r="Q25" s="21"/>
+      <c r="R25" s="21"/>
+      <c r="S25" s="21"/>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26" s="20" t="s">
-        <v>129</v>
+        <v>110</v>
       </c>
       <c r="B26" s="21"/>
       <c r="C26" s="20"/>
       <c r="D26" s="21" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E26" s="21"/>
       <c r="F26" s="21"/>
-      <c r="G26" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="H26" s="21"/>
-      <c r="I26" s="21" t="s">
+      <c r="G26" s="21"/>
+      <c r="H26" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="I26" s="21"/>
+      <c r="J26" s="21"/>
+      <c r="K26" s="21"/>
+      <c r="L26" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="J26" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="K26" s="21"/>
-      <c r="L26" s="21"/>
-      <c r="M26" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="N26" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="O26" s="21" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15">
+      <c r="M26" s="21"/>
+      <c r="N26" s="21"/>
+      <c r="O26" s="21"/>
+      <c r="P26" s="21"/>
+      <c r="Q26" s="21"/>
+      <c r="R26" s="21"/>
+      <c r="S26" s="21"/>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" s="20" t="s">
-        <v>131</v>
+        <v>111</v>
       </c>
       <c r="B27" s="21"/>
       <c r="C27" s="20"/>
       <c r="D27" s="21" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E27" s="21"/>
-      <c r="F27" s="21" t="s">
-        <v>52</v>
-      </c>
+      <c r="F27" s="21"/>
       <c r="G27" s="21"/>
-      <c r="H27" s="21"/>
-      <c r="I27" s="21" t="s">
-        <v>21</v>
-      </c>
+      <c r="H27" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="I27" s="21"/>
       <c r="J27" s="21"/>
       <c r="K27" s="21"/>
-      <c r="L27" s="21"/>
+      <c r="L27" s="21" t="s">
+        <v>67</v>
+      </c>
       <c r="M27" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="N27" s="21" t="s">
-        <v>52</v>
-      </c>
+      <c r="N27" s="21"/>
       <c r="O27" s="21"/>
-    </row>
-    <row r="28" spans="1:15">
+      <c r="P27" s="21"/>
+      <c r="Q27" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="R27" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="S27" s="21"/>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28" s="20" t="s">
-        <v>132</v>
+        <v>112</v>
       </c>
       <c r="B28" s="21"/>
       <c r="C28" s="20"/>
       <c r="D28" s="21" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E28" s="21"/>
-      <c r="F28" s="21" t="s">
-        <v>52</v>
-      </c>
+      <c r="F28" s="21"/>
       <c r="G28" s="21"/>
-      <c r="H28" s="21"/>
-      <c r="I28" s="21" t="s">
-        <v>21</v>
-      </c>
+      <c r="H28" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="I28" s="21"/>
       <c r="J28" s="21"/>
       <c r="K28" s="21"/>
-      <c r="L28" s="21"/>
-      <c r="M28" s="21"/>
+      <c r="L28" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="M28" s="21" t="s">
+        <v>52</v>
+      </c>
       <c r="N28" s="21"/>
       <c r="O28" s="21"/>
-    </row>
-    <row r="29" spans="1:15">
-      <c r="A29" s="20" t="s">
-        <v>133</v>
-      </c>
+      <c r="P28" s="21"/>
+      <c r="Q28" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="R28" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="S28" s="21"/>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A29" s="20"/>
       <c r="B29" s="21"/>
       <c r="C29" s="20"/>
-      <c r="D29" s="21" t="s">
-        <v>100</v>
-      </c>
+      <c r="D29" s="21"/>
       <c r="E29" s="21"/>
-      <c r="F29" s="21" t="s">
-        <v>52</v>
-      </c>
+      <c r="F29" s="21"/>
       <c r="G29" s="21"/>
       <c r="H29" s="21"/>
-      <c r="I29" s="21" t="s">
-        <v>21</v>
-      </c>
+      <c r="I29" s="21"/>
       <c r="J29" s="21"/>
       <c r="K29" s="21"/>
       <c r="L29" s="21"/>
-      <c r="M29" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="N29" s="21" t="s">
-        <v>52</v>
-      </c>
+      <c r="M29" s="21"/>
+      <c r="N29" s="21"/>
       <c r="O29" s="21"/>
-    </row>
-    <row r="30" spans="1:15">
-      <c r="A30" s="20" t="s">
-        <v>134</v>
-      </c>
+      <c r="P29" s="21"/>
+      <c r="Q29" s="21"/>
+      <c r="R29" s="21"/>
+      <c r="S29" s="21"/>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A30" s="20"/>
       <c r="B30" s="21"/>
       <c r="C30" s="20"/>
-      <c r="D30" s="21" t="s">
-        <v>100</v>
-      </c>
+      <c r="D30" s="21"/>
       <c r="E30" s="21"/>
-      <c r="F30" s="21" t="s">
-        <v>52</v>
-      </c>
+      <c r="F30" s="21"/>
       <c r="G30" s="21"/>
       <c r="H30" s="21"/>
-      <c r="I30" s="21" t="s">
-        <v>21</v>
-      </c>
+      <c r="I30" s="21"/>
       <c r="J30" s="21"/>
       <c r="K30" s="21"/>
       <c r="L30" s="21"/>
-      <c r="M30" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="N30" s="21" t="s">
-        <v>52</v>
-      </c>
+      <c r="M30" s="21"/>
+      <c r="N30" s="21"/>
       <c r="O30" s="21"/>
-    </row>
-    <row r="31" spans="1:15">
-      <c r="A31" s="20"/>
+      <c r="P30" s="21"/>
+      <c r="Q30" s="21"/>
+      <c r="R30" s="21"/>
+      <c r="S30" s="21"/>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A31" s="20" t="s">
+        <v>101</v>
+      </c>
       <c r="B31" s="21"/>
       <c r="C31" s="20"/>
-      <c r="D31" s="21"/>
+      <c r="D31" s="21" t="s">
+        <v>102</v>
+      </c>
       <c r="E31" s="21"/>
       <c r="F31" s="21"/>
-      <c r="G31" s="21"/>
-      <c r="H31" s="21"/>
+      <c r="G31" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="H31" s="21" t="s">
+        <v>52</v>
+      </c>
       <c r="I31" s="21"/>
       <c r="J31" s="21"/>
       <c r="K31" s="21"/>
-      <c r="L31" s="21"/>
-      <c r="M31" s="21"/>
+      <c r="L31" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="M31" s="21" t="s">
+        <v>52</v>
+      </c>
       <c r="N31" s="21"/>
       <c r="O31" s="21"/>
-    </row>
-    <row r="32" spans="1:15">
-      <c r="A32" s="20"/>
+      <c r="P31" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q31" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="R31" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="S31" s="21"/>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A32" s="20" t="s">
+        <v>185</v>
+      </c>
       <c r="B32" s="21"/>
       <c r="C32" s="20"/>
-      <c r="D32" s="21"/>
+      <c r="D32" s="21" t="s">
+        <v>102</v>
+      </c>
       <c r="E32" s="21"/>
       <c r="F32" s="21"/>
-      <c r="G32" s="21"/>
+      <c r="G32" s="21" t="s">
+        <v>52</v>
+      </c>
       <c r="H32" s="21"/>
       <c r="I32" s="21"/>
       <c r="J32" s="21"/>
       <c r="K32" s="21"/>
-      <c r="L32" s="21"/>
+      <c r="L32" s="21" t="s">
+        <v>21</v>
+      </c>
       <c r="M32" s="21"/>
       <c r="N32" s="21"/>
       <c r="O32" s="21"/>
-    </row>
-    <row r="33" spans="1:15">
-      <c r="A33" s="20"/>
+      <c r="P32" s="21"/>
+      <c r="Q32" s="21"/>
+      <c r="R32" s="21"/>
+      <c r="S32" s="21"/>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A33" s="20" t="s">
+        <v>103</v>
+      </c>
       <c r="B33" s="21"/>
       <c r="C33" s="20"/>
-      <c r="D33" s="21"/>
+      <c r="D33" s="21" t="s">
+        <v>102</v>
+      </c>
       <c r="E33" s="21"/>
       <c r="F33" s="21"/>
-      <c r="G33" s="21"/>
-      <c r="H33" s="21"/>
+      <c r="G33" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="H33" s="21" t="s">
+        <v>52</v>
+      </c>
       <c r="I33" s="21"/>
       <c r="J33" s="21"/>
       <c r="K33" s="21"/>
-      <c r="L33" s="21"/>
+      <c r="L33" s="21" t="s">
+        <v>21</v>
+      </c>
       <c r="M33" s="21"/>
       <c r="N33" s="21"/>
       <c r="O33" s="21"/>
-    </row>
-    <row r="34" spans="1:15">
-      <c r="A34" s="20"/>
+      <c r="P33" s="21"/>
+      <c r="Q33" s="21"/>
+      <c r="R33" s="21"/>
+      <c r="S33" s="21"/>
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A34" s="20" t="s">
+        <v>113</v>
+      </c>
       <c r="B34" s="21"/>
       <c r="C34" s="20"/>
-      <c r="D34" s="21"/>
+      <c r="D34" s="21" t="s">
+        <v>102</v>
+      </c>
       <c r="E34" s="21"/>
       <c r="F34" s="21"/>
       <c r="G34" s="21"/>
-      <c r="H34" s="21"/>
+      <c r="H34" s="21" t="s">
+        <v>52</v>
+      </c>
       <c r="I34" s="21"/>
       <c r="J34" s="21"/>
       <c r="K34" s="21"/>
-      <c r="L34" s="21"/>
+      <c r="L34" s="21" t="s">
+        <v>67</v>
+      </c>
       <c r="M34" s="21"/>
       <c r="N34" s="21"/>
       <c r="O34" s="21"/>
-    </row>
-    <row r="35" spans="1:15">
-      <c r="A35" s="20"/>
+      <c r="P34" s="21"/>
+      <c r="Q34" s="21"/>
+      <c r="R34" s="21"/>
+      <c r="S34" s="21"/>
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A35" s="20" t="s">
+        <v>200</v>
+      </c>
       <c r="B35" s="21"/>
       <c r="C35" s="20"/>
-      <c r="D35" s="21"/>
+      <c r="D35" s="21" t="s">
+        <v>114</v>
+      </c>
       <c r="E35" s="21"/>
-      <c r="F35" s="21"/>
-      <c r="G35" s="21"/>
+      <c r="F35" s="21">
+        <v>3</v>
+      </c>
+      <c r="G35" s="21" t="s">
+        <v>52</v>
+      </c>
       <c r="H35" s="21"/>
       <c r="I35" s="21"/>
       <c r="J35" s="21"/>
       <c r="K35" s="21"/>
-      <c r="L35" s="21"/>
-      <c r="M35" s="21"/>
-      <c r="N35" s="21"/>
+      <c r="L35" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="M35" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="N35" s="21" t="s">
+        <v>52</v>
+      </c>
       <c r="O35" s="21"/>
-    </row>
-    <row r="36" spans="1:15">
-      <c r="A36" s="20"/>
-      <c r="D36" s="21"/>
+      <c r="P35" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q35" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="R35" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="S35" s="21" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A36" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="B36" s="21"/>
+      <c r="C36" s="20"/>
+      <c r="D36" s="21" t="s">
+        <v>102</v>
+      </c>
       <c r="E36" s="21"/>
       <c r="F36" s="21"/>
-      <c r="G36" s="21"/>
-      <c r="H36" s="21"/>
+      <c r="G36" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="H36" s="21" t="s">
+        <v>52</v>
+      </c>
       <c r="I36" s="21"/>
       <c r="J36" s="21"/>
       <c r="K36" s="21"/>
-      <c r="L36" s="21"/>
+      <c r="L36" s="21" t="s">
+        <v>117</v>
+      </c>
       <c r="M36" s="21"/>
       <c r="N36" s="21"/>
       <c r="O36" s="21"/>
+      <c r="P36" s="21"/>
+      <c r="Q36" s="21"/>
+      <c r="R36" s="21"/>
+      <c r="S36" s="21" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A37" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="B37" s="21"/>
+      <c r="C37" s="20"/>
+      <c r="D37" s="21" t="s">
+        <v>102</v>
+      </c>
+      <c r="E37" s="21"/>
+      <c r="F37" s="21"/>
+      <c r="G37" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="H37" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="I37" s="21"/>
+      <c r="J37" s="21"/>
+      <c r="K37" s="21"/>
+      <c r="L37" s="21" t="s">
+        <v>120</v>
+      </c>
+      <c r="M37" s="21"/>
+      <c r="N37" s="21"/>
+      <c r="O37" s="21"/>
+      <c r="P37" s="21"/>
+      <c r="Q37" s="21"/>
+      <c r="R37" s="21"/>
+      <c r="S37" s="21" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A38" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="B38" s="21"/>
+      <c r="C38" s="20"/>
+      <c r="D38" s="21" t="s">
+        <v>102</v>
+      </c>
+      <c r="E38" s="21"/>
+      <c r="F38" s="21"/>
+      <c r="G38" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="H38" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="I38" s="21"/>
+      <c r="J38" s="21"/>
+      <c r="K38" s="21"/>
+      <c r="L38" s="21" t="s">
+        <v>122</v>
+      </c>
+      <c r="M38" s="21"/>
+      <c r="N38" s="21"/>
+      <c r="O38" s="21"/>
+      <c r="P38" s="21"/>
+      <c r="Q38" s="21"/>
+      <c r="R38" s="21"/>
+      <c r="S38" s="21" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A39" s="20" t="s">
+        <v>123</v>
+      </c>
+      <c r="B39" s="21"/>
+      <c r="C39" s="20"/>
+      <c r="D39" s="21" t="s">
+        <v>102</v>
+      </c>
+      <c r="E39" s="21"/>
+      <c r="F39" s="21"/>
+      <c r="G39" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="H39" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="I39" s="21"/>
+      <c r="J39" s="21"/>
+      <c r="K39" s="21"/>
+      <c r="L39" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="M39" s="21"/>
+      <c r="N39" s="21"/>
+      <c r="O39" s="21"/>
+      <c r="P39" s="21"/>
+      <c r="Q39" s="21"/>
+      <c r="R39" s="21"/>
+      <c r="S39" s="21"/>
+    </row>
+    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A46" s="20"/>
+      <c r="B46" s="21"/>
+      <c r="C46" s="20"/>
+      <c r="D46" s="21"/>
+      <c r="E46" s="21"/>
+      <c r="F46" s="21"/>
+      <c r="G46" s="21"/>
+      <c r="H46" s="21"/>
+      <c r="I46" s="21"/>
+      <c r="J46" s="21"/>
+      <c r="K46" s="21"/>
+      <c r="L46" s="21"/>
+      <c r="M46" s="21"/>
+      <c r="N46" s="21"/>
+      <c r="O46" s="21"/>
+      <c r="P46" s="21"/>
+      <c r="Q46" s="21"/>
+      <c r="R46" s="21"/>
+      <c r="S46" s="21"/>
+    </row>
+    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A47" s="20"/>
+      <c r="B47" s="21"/>
+      <c r="C47" s="20"/>
+      <c r="D47" s="21"/>
+      <c r="E47" s="21"/>
+      <c r="F47" s="21"/>
+      <c r="G47" s="21"/>
+      <c r="H47" s="21"/>
+      <c r="I47" s="21"/>
+      <c r="J47" s="21"/>
+      <c r="K47" s="21"/>
+      <c r="L47" s="21"/>
+      <c r="M47" s="21"/>
+      <c r="N47" s="21"/>
+      <c r="O47" s="21"/>
+      <c r="P47" s="21"/>
+      <c r="Q47" s="21"/>
+      <c r="R47" s="21"/>
+      <c r="S47" s="21"/>
+    </row>
+    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A48" s="20"/>
+      <c r="B48" s="21"/>
+      <c r="C48" s="20"/>
+      <c r="D48" s="21"/>
+      <c r="E48" s="21"/>
+      <c r="F48" s="21"/>
+      <c r="G48" s="21"/>
+      <c r="H48" s="21"/>
+      <c r="I48" s="21"/>
+      <c r="J48" s="21"/>
+      <c r="K48" s="21"/>
+      <c r="L48" s="21"/>
+      <c r="M48" s="21"/>
+      <c r="N48" s="21"/>
+      <c r="O48" s="21"/>
+      <c r="P48" s="21"/>
+      <c r="Q48" s="21"/>
+      <c r="R48" s="21"/>
+      <c r="S48" s="21"/>
+    </row>
+    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A49" s="20"/>
+      <c r="B49" s="21"/>
+      <c r="C49" s="20"/>
+      <c r="D49" s="21"/>
+      <c r="E49" s="21"/>
+      <c r="F49" s="21"/>
+      <c r="G49" s="21"/>
+      <c r="H49" s="21"/>
+      <c r="I49" s="21"/>
+      <c r="J49" s="21"/>
+      <c r="K49" s="21"/>
+      <c r="L49" s="21"/>
+      <c r="M49" s="21"/>
+      <c r="N49" s="21"/>
+      <c r="O49" s="21"/>
+      <c r="P49" s="21"/>
+      <c r="Q49" s="21"/>
+      <c r="R49" s="21"/>
+      <c r="S49" s="21"/>
+    </row>
+    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A50" s="20"/>
+      <c r="B50" s="21"/>
+      <c r="C50" s="20"/>
+      <c r="D50" s="21"/>
+      <c r="E50" s="21"/>
+      <c r="F50" s="21"/>
+      <c r="G50" s="21"/>
+      <c r="H50" s="21"/>
+      <c r="I50" s="21"/>
+      <c r="J50" s="21"/>
+      <c r="K50" s="21"/>
+      <c r="L50" s="21"/>
+      <c r="M50" s="21"/>
+      <c r="N50" s="21"/>
+      <c r="O50" s="21"/>
+      <c r="P50" s="21"/>
+      <c r="Q50" s="21"/>
+      <c r="R50" s="21"/>
+      <c r="S50" s="21"/>
+    </row>
+    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A51" s="20"/>
+      <c r="D51" s="21"/>
+      <c r="E51" s="21"/>
+      <c r="F51" s="21"/>
+      <c r="G51" s="21"/>
+      <c r="H51" s="21"/>
+      <c r="I51" s="21"/>
+      <c r="J51" s="21"/>
+      <c r="K51" s="21"/>
+      <c r="L51" s="21"/>
+      <c r="M51" s="21"/>
+      <c r="N51" s="21"/>
+      <c r="O51" s="21"/>
+      <c r="P51" s="21"/>
+      <c r="Q51" s="21"/>
+      <c r="R51" s="21"/>
+      <c r="S51" s="21"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:O1">
-    <filterColumn colId="1"/>
-    <filterColumn colId="2"/>
-    <filterColumn colId="4"/>
-  </autoFilter>
+  <autoFilter ref="A1:S1"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="38" t="s">
+        <v>189</v>
+      </c>
+      <c r="B1" s="48" t="s">
+        <v>225</v>
+      </c>
+      <c r="C1" s="49"/>
+      <c r="D1" s="48" t="s">
+        <v>226</v>
+      </c>
+      <c r="E1" s="49"/>
+      <c r="F1" s="48" t="s">
+        <v>227</v>
+      </c>
+      <c r="G1" s="49"/>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="27" t="s">
+        <v>190</v>
+      </c>
+      <c r="B2" s="50"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="51" t="s">
+        <v>186</v>
+      </c>
+      <c r="B3" s="40" t="s">
         <v>191</v>
       </c>
-      <c r="B1" s="39">
-        <v>0.01</v>
-      </c>
-      <c r="C1" s="40"/>
-      <c r="D1" s="39">
-        <v>0.2</v>
-      </c>
-      <c r="E1" s="40"/>
-      <c r="F1" s="39">
-        <v>0.4</v>
-      </c>
-      <c r="G1" s="40"/>
-      <c r="H1" s="39">
-        <v>0.6</v>
-      </c>
-      <c r="I1" s="40"/>
-      <c r="J1" s="39">
-        <v>0.8</v>
-      </c>
-      <c r="K1" s="40"/>
-    </row>
-    <row r="2" spans="1:11" ht="15.75" thickBot="1">
-      <c r="A2" s="27" t="s">
+      <c r="C3" s="41"/>
+      <c r="D3" s="40" t="s">
+        <v>191</v>
+      </c>
+      <c r="E3" s="41"/>
+      <c r="F3" s="40" t="s">
+        <v>191</v>
+      </c>
+      <c r="G3" s="41"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="51"/>
+      <c r="B4" s="42" t="s">
         <v>192</v>
       </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
-      <c r="J2" s="43"/>
-      <c r="K2" s="43"/>
-    </row>
-    <row r="3" spans="1:11">
-      <c r="A3" s="42" t="s">
+      <c r="C4" s="43"/>
+      <c r="D4" s="42" t="s">
+        <v>192</v>
+      </c>
+      <c r="E4" s="43"/>
+      <c r="F4" s="42" t="s">
+        <v>192</v>
+      </c>
+      <c r="G4" s="43"/>
+    </row>
+    <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="51"/>
+      <c r="B5" s="44" t="s">
+        <v>193</v>
+      </c>
+      <c r="C5" s="45"/>
+      <c r="D5" s="44" t="s">
+        <v>193</v>
+      </c>
+      <c r="E5" s="45"/>
+      <c r="F5" s="44" t="s">
+        <v>193</v>
+      </c>
+      <c r="G5" s="45"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="51" t="s">
+        <v>187</v>
+      </c>
+      <c r="B6" s="40" t="s">
+        <v>191</v>
+      </c>
+      <c r="C6" s="41"/>
+      <c r="D6" s="40" t="s">
+        <v>191</v>
+      </c>
+      <c r="E6" s="46"/>
+      <c r="F6" s="40" t="s">
+        <v>191</v>
+      </c>
+      <c r="G6" s="41"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="51"/>
+      <c r="B7" s="42" t="s">
+        <v>192</v>
+      </c>
+      <c r="C7" s="43"/>
+      <c r="D7" s="42" t="s">
+        <v>192</v>
+      </c>
+      <c r="E7" s="39"/>
+      <c r="F7" s="42" t="s">
+        <v>192</v>
+      </c>
+      <c r="G7" s="43"/>
+    </row>
+    <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="51"/>
+      <c r="B8" s="44" t="s">
+        <v>193</v>
+      </c>
+      <c r="C8" s="45"/>
+      <c r="D8" s="44" t="s">
+        <v>193</v>
+      </c>
+      <c r="E8" s="47"/>
+      <c r="F8" s="44" t="s">
+        <v>193</v>
+      </c>
+      <c r="G8" s="45"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="51" t="s">
         <v>188</v>
       </c>
-      <c r="B3" s="44" t="s">
+      <c r="B9" s="40" t="s">
+        <v>191</v>
+      </c>
+      <c r="C9" s="41"/>
+      <c r="D9" s="40" t="s">
+        <v>191</v>
+      </c>
+      <c r="E9" s="41"/>
+      <c r="F9" s="40" t="s">
+        <v>191</v>
+      </c>
+      <c r="G9" s="41"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="51"/>
+      <c r="B10" s="42" t="s">
+        <v>192</v>
+      </c>
+      <c r="C10" s="43"/>
+      <c r="D10" s="42" t="s">
+        <v>192</v>
+      </c>
+      <c r="E10" s="43"/>
+      <c r="F10" s="42" t="s">
+        <v>192</v>
+      </c>
+      <c r="G10" s="43"/>
+    </row>
+    <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="51"/>
+      <c r="B11" s="44" t="s">
         <v>193</v>
       </c>
-      <c r="C3" s="45"/>
-      <c r="D3" s="44" t="s">
+      <c r="C11" s="45"/>
+      <c r="D11" s="44" t="s">
         <v>193</v>
       </c>
-      <c r="E3" s="45"/>
-      <c r="F3" s="44" t="s">
+      <c r="E11" s="45"/>
+      <c r="F11" s="44" t="s">
         <v>193</v>
       </c>
-      <c r="G3" s="45"/>
-      <c r="H3" s="44" t="s">
-        <v>193</v>
-      </c>
-      <c r="I3" s="45"/>
-      <c r="J3" s="44" t="s">
-        <v>193</v>
-      </c>
-      <c r="K3" s="45"/>
-    </row>
-    <row r="4" spans="1:11">
-      <c r="A4" s="42"/>
-      <c r="B4" s="46" t="s">
-        <v>194</v>
-      </c>
-      <c r="C4" s="47"/>
-      <c r="D4" s="46" t="s">
-        <v>194</v>
-      </c>
-      <c r="E4" s="47"/>
-      <c r="F4" s="46" t="s">
-        <v>194</v>
-      </c>
-      <c r="G4" s="47"/>
-      <c r="H4" s="46" t="s">
-        <v>194</v>
-      </c>
-      <c r="I4" s="47"/>
-      <c r="J4" s="46" t="s">
-        <v>194</v>
-      </c>
-      <c r="K4" s="47"/>
-    </row>
-    <row r="5" spans="1:11" ht="15.75" thickBot="1">
-      <c r="A5" s="42"/>
-      <c r="B5" s="48" t="s">
-        <v>195</v>
-      </c>
-      <c r="C5" s="49"/>
-      <c r="D5" s="48" t="s">
-        <v>195</v>
-      </c>
-      <c r="E5" s="49"/>
-      <c r="F5" s="48" t="s">
-        <v>195</v>
-      </c>
-      <c r="G5" s="49"/>
-      <c r="H5" s="48" t="s">
-        <v>195</v>
-      </c>
-      <c r="I5" s="49"/>
-      <c r="J5" s="48" t="s">
-        <v>195</v>
-      </c>
-      <c r="K5" s="49"/>
-    </row>
-    <row r="6" spans="1:11">
-      <c r="A6" s="42" t="s">
-        <v>189</v>
-      </c>
-      <c r="B6" s="44" t="s">
-        <v>193</v>
-      </c>
-      <c r="C6" s="45"/>
-      <c r="D6" s="44" t="s">
-        <v>193</v>
-      </c>
-      <c r="E6" s="50"/>
-      <c r="F6" s="44" t="s">
-        <v>193</v>
-      </c>
-      <c r="G6" s="45"/>
-      <c r="H6" s="44" t="s">
-        <v>193</v>
-      </c>
-      <c r="I6" s="45"/>
-      <c r="J6" s="44" t="s">
-        <v>193</v>
-      </c>
-      <c r="K6" s="45"/>
-    </row>
-    <row r="7" spans="1:11">
-      <c r="A7" s="42"/>
-      <c r="B7" s="46" t="s">
-        <v>194</v>
-      </c>
-      <c r="C7" s="47"/>
-      <c r="D7" s="46" t="s">
-        <v>194</v>
-      </c>
-      <c r="E7" s="41"/>
-      <c r="F7" s="46" t="s">
-        <v>194</v>
-      </c>
-      <c r="G7" s="47"/>
-      <c r="H7" s="46" t="s">
-        <v>194</v>
-      </c>
-      <c r="I7" s="47"/>
-      <c r="J7" s="46" t="s">
-        <v>194</v>
-      </c>
-      <c r="K7" s="47"/>
-    </row>
-    <row r="8" spans="1:11" ht="15.75" thickBot="1">
-      <c r="A8" s="42"/>
-      <c r="B8" s="48" t="s">
-        <v>195</v>
-      </c>
-      <c r="C8" s="49"/>
-      <c r="D8" s="48" t="s">
-        <v>195</v>
-      </c>
-      <c r="E8" s="51"/>
-      <c r="F8" s="48" t="s">
-        <v>195</v>
-      </c>
-      <c r="G8" s="49"/>
-      <c r="H8" s="48" t="s">
-        <v>195</v>
-      </c>
-      <c r="I8" s="49"/>
-      <c r="J8" s="48" t="s">
-        <v>195</v>
-      </c>
-      <c r="K8" s="49"/>
-    </row>
-    <row r="9" spans="1:11">
-      <c r="A9" s="42" t="s">
-        <v>190</v>
-      </c>
-      <c r="B9" s="44" t="s">
-        <v>193</v>
-      </c>
-      <c r="C9" s="45"/>
-      <c r="D9" s="44" t="s">
-        <v>193</v>
-      </c>
-      <c r="E9" s="45"/>
-      <c r="F9" s="44" t="s">
-        <v>193</v>
-      </c>
-      <c r="G9" s="45"/>
-      <c r="H9" s="44" t="s">
-        <v>193</v>
-      </c>
-      <c r="I9" s="45"/>
-      <c r="J9" s="44" t="s">
-        <v>193</v>
-      </c>
-      <c r="K9" s="45"/>
-    </row>
-    <row r="10" spans="1:11">
-      <c r="A10" s="42"/>
-      <c r="B10" s="46" t="s">
-        <v>194</v>
-      </c>
-      <c r="C10" s="47"/>
-      <c r="D10" s="46" t="s">
-        <v>194</v>
-      </c>
-      <c r="E10" s="47"/>
-      <c r="F10" s="46" t="s">
-        <v>194</v>
-      </c>
-      <c r="G10" s="47"/>
-      <c r="H10" s="46" t="s">
-        <v>194</v>
-      </c>
-      <c r="I10" s="47"/>
-      <c r="J10" s="46" t="s">
-        <v>194</v>
-      </c>
-      <c r="K10" s="47"/>
-    </row>
-    <row r="11" spans="1:11" ht="15.75" thickBot="1">
-      <c r="A11" s="42"/>
-      <c r="B11" s="48" t="s">
-        <v>195</v>
-      </c>
-      <c r="C11" s="49"/>
-      <c r="D11" s="48" t="s">
-        <v>195</v>
-      </c>
-      <c r="E11" s="49"/>
-      <c r="F11" s="48" t="s">
-        <v>195</v>
-      </c>
-      <c r="G11" s="49"/>
-      <c r="H11" s="48" t="s">
-        <v>195</v>
-      </c>
-      <c r="I11" s="49"/>
-      <c r="J11" s="48" t="s">
-        <v>195</v>
-      </c>
-      <c r="K11" s="49"/>
+      <c r="G11" s="45"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="H1:I2"/>
-    <mergeCell ref="J1:K2"/>
+  <mergeCells count="6">
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="A6:A8"/>
     <mergeCell ref="A9:A11"/>
@@ -4584,65 +5034,70 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:U2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:U7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="12" width="11.42578125" style="9"/>
     <col min="13" max="13" width="12.85546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="14" max="21" width="11.42578125" style="9"/>
+    <col min="14" max="18" width="11.42578125" style="9"/>
+    <col min="19" max="19" width="14.85546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.42578125" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="20" customFormat="1">
+    <row r="1" spans="1:21" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="32" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C1" s="32" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D1" s="28" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E1" s="28" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="F1" s="28" t="s">
-        <v>153</v>
-      </c>
-      <c r="G1" s="28"/>
+        <v>151</v>
+      </c>
+      <c r="G1" s="28" t="s">
+        <v>149</v>
+      </c>
       <c r="H1" s="28"/>
       <c r="I1" s="28"/>
       <c r="J1" s="28"/>
@@ -4664,25 +5119,27 @@
         <v>13</v>
       </c>
       <c r="R1" s="30" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="S1" s="30" t="s">
-        <v>15</v>
-      </c>
-      <c r="T1" s="31" t="s">
-        <v>16</v>
-      </c>
-      <c r="U1" s="21"/>
-    </row>
-    <row r="2" spans="1:21">
+        <v>213</v>
+      </c>
+      <c r="T1" s="30" t="s">
+        <v>213</v>
+      </c>
+      <c r="U1" s="30" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B2" s="9">
         <v>1</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D2" s="9">
         <v>4</v>
@@ -4694,13 +5151,185 @@
         <v>22</v>
       </c>
       <c r="O2" s="9" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="Q2" s="9">
         <v>1</v>
       </c>
       <c r="R2" s="9">
         <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>211</v>
+      </c>
+      <c r="B3" s="9">
+        <v>1</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="D3" s="9">
+        <v>0</v>
+      </c>
+      <c r="E3" s="37">
+        <v>0.2</v>
+      </c>
+      <c r="M3" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="N3" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="O3" s="9">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="9">
+        <v>1</v>
+      </c>
+      <c r="S3" s="9" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>215</v>
+      </c>
+      <c r="B4" s="9">
+        <v>2</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="D4" s="9">
+        <v>6</v>
+      </c>
+      <c r="E4" s="37">
+        <v>0.05</v>
+      </c>
+      <c r="M4" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="N4" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="O4" s="9">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="9">
+        <v>1</v>
+      </c>
+      <c r="S4" s="9" t="s">
+        <v>214</v>
+      </c>
+      <c r="T4" s="9" t="s">
+        <v>216</v>
+      </c>
+      <c r="U4" s="9" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>218</v>
+      </c>
+      <c r="B5" s="9">
+        <v>2</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="D5" s="9">
+        <v>0</v>
+      </c>
+      <c r="G5" s="9">
+        <v>1</v>
+      </c>
+      <c r="M5" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="N5" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="O5" s="9">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="9">
+        <v>2</v>
+      </c>
+      <c r="R5" s="9">
+        <v>5</v>
+      </c>
+      <c r="S5" s="9" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>221</v>
+      </c>
+      <c r="B6" s="9">
+        <v>2</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="D6" s="9">
+        <v>2</v>
+      </c>
+      <c r="E6" s="37">
+        <v>0.1</v>
+      </c>
+      <c r="N6" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="O6" s="9">
+        <v>1</v>
+      </c>
+      <c r="Q6" s="9">
+        <v>0</v>
+      </c>
+      <c r="S6" s="9" t="s">
+        <v>214</v>
+      </c>
+      <c r="T6" s="9" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>222</v>
+      </c>
+      <c r="B7" s="9">
+        <v>2</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="D7" s="9">
+        <v>0</v>
+      </c>
+      <c r="G7" s="9">
+        <v>3</v>
+      </c>
+      <c r="N7" s="9" t="s">
+        <v>223</v>
+      </c>
+      <c r="O7" s="9">
+        <v>1</v>
+      </c>
+      <c r="Q7" s="9">
+        <v>2</v>
+      </c>
+      <c r="R7" s="9">
+        <v>5</v>
+      </c>
+      <c r="S7" s="9" t="s">
+        <v>219</v>
+      </c>
+      <c r="T7" s="9" t="s">
+        <v>184</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Assets Map Tile (1)
</commit_message>
<xml_diff>
--- a/Game Design/Assets.xlsx
+++ b/Game Design/Assets.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="105" windowWidth="15120" windowHeight="8010" activeTab="4"/>
+    <workbookView xWindow="120" yWindow="105" windowWidth="15120" windowHeight="8010" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Weapons" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="639" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="681" uniqueCount="247">
   <si>
     <t>Name</t>
   </si>
@@ -715,13 +715,70 @@
   </si>
   <si>
     <t>Wet</t>
+  </si>
+  <si>
+    <t>Rock Desrt</t>
+  </si>
+  <si>
+    <t>Rock Wasteland</t>
+  </si>
+  <si>
+    <t>Ice Mountain</t>
+  </si>
+  <si>
+    <t>Ice Wasteland</t>
+  </si>
+  <si>
+    <t>Forest Mountain</t>
+  </si>
+  <si>
+    <t>Snow Forest</t>
+  </si>
+  <si>
+    <t>Ice Forest</t>
+  </si>
+  <si>
+    <t>Jungle</t>
+  </si>
+  <si>
+    <t>Jungle Mauntain</t>
+  </si>
+  <si>
+    <t>Forest Mauntain</t>
+  </si>
+  <si>
+    <t>Bush Forest Mountain</t>
+  </si>
+  <si>
+    <t>Snow Forest Mountain</t>
+  </si>
+  <si>
+    <t>Ice Forest Mauntain</t>
+  </si>
+  <si>
+    <t>Bush Forest</t>
+  </si>
+  <si>
+    <t>Dry Grassland</t>
+  </si>
+  <si>
+    <t>Bush Grassland</t>
+  </si>
+  <si>
+    <t>Dry Wasteland</t>
+  </si>
+  <si>
+    <t>Mountain Wasteland</t>
+  </si>
+  <si>
+    <t>Sand Desert</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -779,8 +836,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="13">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -846,6 +910,16 @@
       <patternFill patternType="solid">
         <fgColor theme="0"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
       </patternFill>
     </fill>
   </fills>
@@ -1138,7 +1212,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1146,8 +1220,10 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
@@ -1242,14 +1318,14 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="9" fontId="1" fillId="2" borderId="9" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1259,11 +1335,16 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="17" xfId="7" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="15" xfId="8" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="9">
+    <cellStyle name="Akzent1" xfId="7" builtinId="29"/>
+    <cellStyle name="Akzent3" xfId="8" builtinId="37"/>
     <cellStyle name="Ausgabe" xfId="5" builtinId="21"/>
     <cellStyle name="Berechnung" xfId="6" builtinId="22"/>
     <cellStyle name="Eingabe" xfId="4" builtinId="20"/>
@@ -1285,6 +1366,627 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>214313</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>53579</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>500063</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>148829</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Grafik 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="214313" y="4304110"/>
+          <a:ext cx="1047750" cy="1047750"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>77391</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>24271</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>716757</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>121443</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Grafik 14"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="77391" y="2738896"/>
+          <a:ext cx="1401366" cy="1049672"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>142874</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>88396</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>526255</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="Grafik 15"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1666874" y="2803021"/>
+          <a:ext cx="1687115" cy="921254"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>154782</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>68042</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>413147</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>126206</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="Grafik 16"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3744516" y="2782667"/>
+          <a:ext cx="1621631" cy="1010664"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>244079</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>59531</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>294637</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>121443</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="18" name="Grafik 17"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1768079" y="4310062"/>
+          <a:ext cx="1354292" cy="1014412"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>273845</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>67392</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>270272</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="19" name="Grafik 18"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3863579" y="4317923"/>
+          <a:ext cx="1359693" cy="1018458"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>53578</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>56575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>740568</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>89297</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="20" name="Grafik 19"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="53578" y="5831106"/>
+          <a:ext cx="1448990" cy="985222"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>232172</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>50152</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>506016</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>124780</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="21" name="Grafik 20"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1756172" y="5824683"/>
+          <a:ext cx="1577578" cy="1027128"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>136923</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>24614</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>416719</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>165497</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="22" name="Grafik 21"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3726657" y="5799145"/>
+          <a:ext cx="1643062" cy="1093383"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>107156</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>64056</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>593612</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>77391</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="23" name="Grafik 22"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5822156" y="2778681"/>
+          <a:ext cx="1724706" cy="965835"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>65485</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>53577</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>621676</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>105964</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="24" name="Grafik 23"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5780485" y="4304108"/>
+          <a:ext cx="1794441" cy="1004887"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>71437</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>38444</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>550068</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>155972</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="25" name="Grafik 24"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5786437" y="5812975"/>
+          <a:ext cx="1716881" cy="1070028"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>33512</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>140265</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>708422</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>136921</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="26" name="Grafik 25"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7748762" y="2854890"/>
+          <a:ext cx="1436910" cy="758656"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>35720</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>71437</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>730120</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>88105</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="27" name="Grafik 26"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="35720" y="7369968"/>
+          <a:ext cx="1456400" cy="969168"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3342,7 +4044,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
@@ -4843,193 +5545,730 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:L60"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39:D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="38" t="s">
         <v>189</v>
       </c>
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="46" t="s">
         <v>225</v>
       </c>
-      <c r="C1" s="49"/>
-      <c r="D1" s="48" t="s">
+      <c r="C1" s="47"/>
+      <c r="D1" s="46" t="s">
         <v>226</v>
       </c>
-      <c r="E1" s="49"/>
-      <c r="F1" s="48" t="s">
+      <c r="E1" s="47"/>
+      <c r="F1" s="46" t="s">
         <v>227</v>
       </c>
-      <c r="G1" s="49"/>
-    </row>
-    <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G1" s="47"/>
+    </row>
+    <row r="2" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="27" t="s">
         <v>190</v>
       </c>
-      <c r="B2" s="50"/>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50"/>
-      <c r="G2" s="50"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="51" t="s">
+      <c r="B2" s="48"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="48"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="45" t="s">
         <v>186</v>
       </c>
-      <c r="B3" s="40" t="s">
+      <c r="B3" s="51" t="s">
         <v>191</v>
       </c>
-      <c r="C3" s="41"/>
-      <c r="D3" s="40" t="s">
+      <c r="C3" s="40" t="s">
+        <v>229</v>
+      </c>
+      <c r="D3" s="51" t="s">
         <v>191</v>
       </c>
-      <c r="E3" s="41"/>
-      <c r="F3" s="40" t="s">
+      <c r="E3" s="40" t="s">
+        <v>238</v>
+      </c>
+      <c r="F3" s="51" t="s">
         <v>191</v>
       </c>
-      <c r="G3" s="41"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="51"/>
-      <c r="B4" s="42" t="s">
+      <c r="G3" s="40" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="45"/>
+      <c r="B4" s="50" t="s">
         <v>192</v>
       </c>
-      <c r="C4" s="43"/>
-      <c r="D4" s="42" t="s">
+      <c r="C4" s="41" t="s">
+        <v>245</v>
+      </c>
+      <c r="D4" s="50" t="s">
         <v>192</v>
       </c>
-      <c r="E4" s="43"/>
-      <c r="F4" s="42" t="s">
+      <c r="E4" s="41" t="s">
+        <v>232</v>
+      </c>
+      <c r="F4" s="50" t="s">
         <v>192</v>
       </c>
-      <c r="G4" s="43"/>
-    </row>
-    <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="51"/>
-      <c r="B5" s="44" t="s">
+      <c r="G4" s="41" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="45"/>
+      <c r="B5" s="49" t="s">
         <v>193</v>
       </c>
-      <c r="C5" s="45"/>
-      <c r="D5" s="44" t="s">
+      <c r="C5" s="42" t="s">
+        <v>230</v>
+      </c>
+      <c r="D5" s="49" t="s">
         <v>193</v>
       </c>
-      <c r="E5" s="45"/>
-      <c r="F5" s="44" t="s">
+      <c r="E5" s="42" t="s">
+        <v>239</v>
+      </c>
+      <c r="F5" s="49" t="s">
         <v>193</v>
       </c>
-      <c r="G5" s="45"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="51" t="s">
+      <c r="G5" s="42" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="45" t="s">
         <v>187</v>
       </c>
-      <c r="B6" s="40" t="s">
+      <c r="B6" s="51" t="s">
         <v>191</v>
       </c>
-      <c r="C6" s="41"/>
-      <c r="D6" s="40" t="s">
+      <c r="C6" s="40" t="s">
+        <v>228</v>
+      </c>
+      <c r="D6" s="51" t="s">
         <v>191</v>
       </c>
-      <c r="E6" s="46"/>
-      <c r="F6" s="40" t="s">
+      <c r="E6" s="43" t="s">
+        <v>241</v>
+      </c>
+      <c r="F6" s="51" t="s">
         <v>191</v>
       </c>
-      <c r="G6" s="41"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="51"/>
-      <c r="B7" s="42" t="s">
+      <c r="G6" s="40" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="45"/>
+      <c r="B7" s="50" t="s">
         <v>192</v>
       </c>
-      <c r="C7" s="43"/>
-      <c r="D7" s="42" t="s">
+      <c r="C7" s="41" t="s">
+        <v>242</v>
+      </c>
+      <c r="D7" s="50" t="s">
         <v>192</v>
       </c>
-      <c r="E7" s="39"/>
-      <c r="F7" s="42" t="s">
+      <c r="E7" s="39" t="s">
+        <v>165</v>
+      </c>
+      <c r="F7" s="50" t="s">
         <v>192</v>
       </c>
-      <c r="G7" s="43"/>
-    </row>
-    <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="51"/>
-      <c r="B8" s="44" t="s">
+      <c r="G7" s="41" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="45"/>
+      <c r="B8" s="49" t="s">
         <v>193</v>
       </c>
-      <c r="C8" s="45"/>
-      <c r="D8" s="44" t="s">
+      <c r="C8" s="42" t="s">
+        <v>169</v>
+      </c>
+      <c r="D8" s="49" t="s">
         <v>193</v>
       </c>
-      <c r="E8" s="47"/>
-      <c r="F8" s="44" t="s">
+      <c r="E8" s="44" t="s">
+        <v>233</v>
+      </c>
+      <c r="F8" s="49" t="s">
         <v>193</v>
       </c>
-      <c r="G8" s="45"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="51" t="s">
+      <c r="G8" s="42" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="45" t="s">
         <v>188</v>
       </c>
-      <c r="B9" s="40" t="s">
+      <c r="B9" s="51" t="s">
         <v>191</v>
       </c>
-      <c r="C9" s="41"/>
-      <c r="D9" s="40" t="s">
+      <c r="C9" s="40" t="s">
+        <v>246</v>
+      </c>
+      <c r="D9" s="51" t="s">
         <v>191</v>
       </c>
-      <c r="E9" s="41"/>
-      <c r="F9" s="40" t="s">
+      <c r="E9" s="40" t="s">
+        <v>243</v>
+      </c>
+      <c r="F9" s="51" t="s">
         <v>191</v>
       </c>
-      <c r="G9" s="41"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="51"/>
-      <c r="B10" s="42" t="s">
+      <c r="G9" s="40" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="45"/>
+      <c r="B10" s="50" t="s">
         <v>192</v>
       </c>
-      <c r="C10" s="43"/>
-      <c r="D10" s="42" t="s">
+      <c r="C10" s="41" t="s">
+        <v>244</v>
+      </c>
+      <c r="D10" s="50" t="s">
         <v>192</v>
       </c>
-      <c r="E10" s="43"/>
-      <c r="F10" s="42" t="s">
+      <c r="E10" s="41" t="s">
+        <v>224</v>
+      </c>
+      <c r="F10" s="50" t="s">
         <v>192</v>
       </c>
-      <c r="G10" s="43"/>
-    </row>
-    <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="51"/>
-      <c r="B11" s="44" t="s">
+      <c r="G10" s="41" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="45"/>
+      <c r="B11" s="49" t="s">
         <v>193</v>
       </c>
-      <c r="C11" s="45"/>
-      <c r="D11" s="44" t="s">
+      <c r="C11" s="42" t="s">
+        <v>231</v>
+      </c>
+      <c r="D11" s="49" t="s">
         <v>193</v>
       </c>
-      <c r="E11" s="45"/>
-      <c r="F11" s="44" t="s">
+      <c r="E11" s="42" t="s">
+        <v>231</v>
+      </c>
+      <c r="F11" s="49" t="s">
         <v>193</v>
       </c>
-      <c r="G11" s="45"/>
+      <c r="G11" s="42" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>229</v>
+      </c>
+      <c r="C14" t="s">
+        <v>245</v>
+      </c>
+      <c r="E14" t="s">
+        <v>230</v>
+      </c>
+      <c r="G14" t="s">
+        <v>238</v>
+      </c>
+      <c r="I14" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="52"/>
+      <c r="B15" s="52"/>
+      <c r="C15" s="52"/>
+      <c r="D15" s="52"/>
+      <c r="E15" s="52"/>
+      <c r="F15" s="52"/>
+      <c r="G15" s="52"/>
+      <c r="H15" s="52"/>
+      <c r="I15" s="52"/>
+      <c r="J15" s="52"/>
+      <c r="K15" s="52"/>
+      <c r="L15" s="52"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="52"/>
+      <c r="B16" s="52"/>
+      <c r="C16" s="52"/>
+      <c r="D16" s="52"/>
+      <c r="E16" s="52"/>
+      <c r="F16" s="52"/>
+      <c r="G16" s="52"/>
+      <c r="H16" s="52"/>
+      <c r="I16" s="52"/>
+      <c r="J16" s="52"/>
+      <c r="K16" s="52"/>
+      <c r="L16" s="52"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="52"/>
+      <c r="B17" s="52"/>
+      <c r="C17" s="52"/>
+      <c r="D17" s="52"/>
+      <c r="E17" s="52"/>
+      <c r="F17" s="52"/>
+      <c r="G17" s="52"/>
+      <c r="H17" s="52"/>
+      <c r="I17" s="52"/>
+      <c r="J17" s="52"/>
+      <c r="K17" s="52"/>
+      <c r="L17" s="52"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="52"/>
+      <c r="B18" s="52"/>
+      <c r="C18" s="52"/>
+      <c r="D18" s="52"/>
+      <c r="E18" s="52"/>
+      <c r="F18" s="52"/>
+      <c r="G18" s="52"/>
+      <c r="H18" s="52"/>
+      <c r="I18" s="52"/>
+      <c r="J18" s="52"/>
+      <c r="K18" s="52"/>
+      <c r="L18" s="52"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="52"/>
+      <c r="B19" s="52"/>
+      <c r="C19" s="52"/>
+      <c r="D19" s="52"/>
+      <c r="E19" s="52"/>
+      <c r="F19" s="52"/>
+      <c r="G19" s="52"/>
+      <c r="H19" s="52"/>
+      <c r="I19" s="52"/>
+      <c r="J19" s="52"/>
+      <c r="K19" s="52"/>
+      <c r="L19" s="52"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="52"/>
+      <c r="B20" s="52"/>
+      <c r="C20" s="52"/>
+      <c r="D20" s="52"/>
+      <c r="E20" s="52"/>
+      <c r="F20" s="52"/>
+      <c r="G20" s="52"/>
+      <c r="H20" s="52"/>
+      <c r="I20" s="52"/>
+      <c r="J20" s="52"/>
+      <c r="K20" s="52"/>
+      <c r="L20" s="52"/>
+    </row>
+    <row r="21" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" s="40" t="s">
+        <v>228</v>
+      </c>
+      <c r="C22" t="s">
+        <v>242</v>
+      </c>
+      <c r="E22" t="s">
+        <v>169</v>
+      </c>
+      <c r="G22" t="s">
+        <v>232</v>
+      </c>
+      <c r="I22" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" s="52"/>
+      <c r="B23" s="52"/>
+      <c r="C23" s="52"/>
+      <c r="D23" s="52"/>
+      <c r="E23" s="52"/>
+      <c r="F23" s="52"/>
+      <c r="G23" s="52"/>
+      <c r="H23" s="52"/>
+      <c r="I23" s="52"/>
+      <c r="J23" s="52"/>
+      <c r="K23" s="52"/>
+      <c r="L23" s="52"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" s="52"/>
+      <c r="B24" s="52"/>
+      <c r="C24" s="52"/>
+      <c r="D24" s="52"/>
+      <c r="E24" s="52"/>
+      <c r="F24" s="52"/>
+      <c r="G24" s="52"/>
+      <c r="H24" s="52"/>
+      <c r="I24" s="52"/>
+      <c r="J24" s="52"/>
+      <c r="K24" s="52"/>
+      <c r="L24" s="52"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" s="52"/>
+      <c r="B25" s="52"/>
+      <c r="C25" s="52"/>
+      <c r="D25" s="52"/>
+      <c r="E25" s="52"/>
+      <c r="F25" s="52"/>
+      <c r="G25" s="52"/>
+      <c r="H25" s="52"/>
+      <c r="I25" s="52"/>
+      <c r="J25" s="52"/>
+      <c r="K25" s="52"/>
+      <c r="L25" s="52"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" s="52"/>
+      <c r="B26" s="52"/>
+      <c r="C26" s="52"/>
+      <c r="D26" s="52"/>
+      <c r="E26" s="52"/>
+      <c r="F26" s="52"/>
+      <c r="G26" s="52"/>
+      <c r="H26" s="52"/>
+      <c r="I26" s="52"/>
+      <c r="J26" s="52"/>
+      <c r="K26" s="52"/>
+      <c r="L26" s="52"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" s="52"/>
+      <c r="B27" s="52"/>
+      <c r="C27" s="52"/>
+      <c r="D27" s="52"/>
+      <c r="E27" s="52"/>
+      <c r="F27" s="52"/>
+      <c r="G27" s="52"/>
+      <c r="H27" s="52"/>
+      <c r="I27" s="52"/>
+      <c r="J27" s="52"/>
+      <c r="K27" s="52"/>
+      <c r="L27" s="52"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" s="52"/>
+      <c r="B28" s="52"/>
+      <c r="C28" s="52"/>
+      <c r="D28" s="52"/>
+      <c r="E28" s="52"/>
+      <c r="F28" s="52"/>
+      <c r="G28" s="52"/>
+      <c r="H28" s="52"/>
+      <c r="I28" s="52"/>
+      <c r="J28" s="52"/>
+      <c r="K28" s="52"/>
+      <c r="L28" s="52"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>246</v>
+      </c>
+      <c r="C30" t="s">
+        <v>244</v>
+      </c>
+      <c r="E30" t="s">
+        <v>231</v>
+      </c>
+      <c r="G30" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" s="52"/>
+      <c r="B31" s="52"/>
+      <c r="C31" s="52"/>
+      <c r="D31" s="52"/>
+      <c r="E31" s="52"/>
+      <c r="F31" s="52"/>
+      <c r="G31" s="52"/>
+      <c r="H31" s="52"/>
+      <c r="I31" s="52"/>
+      <c r="J31" s="52"/>
+      <c r="K31" s="52"/>
+      <c r="L31" s="52"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32" s="52"/>
+      <c r="B32" s="52"/>
+      <c r="C32" s="52"/>
+      <c r="D32" s="52"/>
+      <c r="E32" s="52"/>
+      <c r="F32" s="52"/>
+      <c r="G32" s="52"/>
+      <c r="H32" s="52"/>
+      <c r="I32" s="52"/>
+      <c r="J32" s="52"/>
+      <c r="K32" s="52"/>
+      <c r="L32" s="52"/>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A33" s="52"/>
+      <c r="B33" s="52"/>
+      <c r="C33" s="52"/>
+      <c r="D33" s="52"/>
+      <c r="E33" s="52"/>
+      <c r="F33" s="52"/>
+      <c r="G33" s="52"/>
+      <c r="H33" s="52"/>
+      <c r="I33" s="52"/>
+      <c r="J33" s="52"/>
+      <c r="K33" s="52"/>
+      <c r="L33" s="52"/>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A34" s="52"/>
+      <c r="B34" s="52"/>
+      <c r="C34" s="52"/>
+      <c r="D34" s="52"/>
+      <c r="E34" s="52"/>
+      <c r="F34" s="52"/>
+      <c r="G34" s="52"/>
+      <c r="H34" s="52"/>
+      <c r="I34" s="52"/>
+      <c r="J34" s="52"/>
+      <c r="K34" s="52"/>
+      <c r="L34" s="52"/>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A35" s="52"/>
+      <c r="B35" s="52"/>
+      <c r="C35" s="52"/>
+      <c r="D35" s="52"/>
+      <c r="E35" s="52"/>
+      <c r="F35" s="52"/>
+      <c r="G35" s="52"/>
+      <c r="H35" s="52"/>
+      <c r="I35" s="52"/>
+      <c r="J35" s="52"/>
+      <c r="K35" s="52"/>
+      <c r="L35" s="52"/>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A36" s="52"/>
+      <c r="B36" s="52"/>
+      <c r="C36" s="52"/>
+      <c r="D36" s="52"/>
+      <c r="E36" s="52"/>
+      <c r="F36" s="52"/>
+      <c r="G36" s="52"/>
+      <c r="H36" s="52"/>
+      <c r="I36" s="52"/>
+      <c r="J36" s="52"/>
+      <c r="K36" s="52"/>
+      <c r="L36" s="52"/>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A39" s="52"/>
+      <c r="B39" s="52"/>
+      <c r="C39" s="52"/>
+      <c r="D39" s="52"/>
+      <c r="E39" s="52"/>
+      <c r="F39" s="52"/>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A40" s="52"/>
+      <c r="B40" s="52"/>
+      <c r="C40" s="52"/>
+      <c r="D40" s="52"/>
+      <c r="E40" s="52"/>
+      <c r="F40" s="52"/>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A41" s="52"/>
+      <c r="B41" s="52"/>
+      <c r="C41" s="52"/>
+      <c r="D41" s="52"/>
+      <c r="E41" s="52"/>
+      <c r="F41" s="52"/>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A42" s="52"/>
+      <c r="B42" s="52"/>
+      <c r="C42" s="52"/>
+      <c r="D42" s="52"/>
+      <c r="E42" s="52"/>
+      <c r="F42" s="52"/>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A43" s="52"/>
+      <c r="B43" s="52"/>
+      <c r="C43" s="52"/>
+      <c r="D43" s="52"/>
+      <c r="E43" s="52"/>
+      <c r="F43" s="52"/>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A44" s="52"/>
+      <c r="B44" s="52"/>
+      <c r="C44" s="52"/>
+      <c r="D44" s="52"/>
+      <c r="E44" s="52"/>
+      <c r="F44" s="52"/>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A47" s="52"/>
+      <c r="B47" s="52"/>
+      <c r="C47" s="52"/>
+      <c r="D47" s="52"/>
+      <c r="E47" s="52"/>
+      <c r="F47" s="52"/>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A48" s="52"/>
+      <c r="B48" s="52"/>
+      <c r="C48" s="52"/>
+      <c r="D48" s="52"/>
+      <c r="E48" s="52"/>
+      <c r="F48" s="52"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="52"/>
+      <c r="B49" s="52"/>
+      <c r="C49" s="52"/>
+      <c r="D49" s="52"/>
+      <c r="E49" s="52"/>
+      <c r="F49" s="52"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="52"/>
+      <c r="B50" s="52"/>
+      <c r="C50" s="52"/>
+      <c r="D50" s="52"/>
+      <c r="E50" s="52"/>
+      <c r="F50" s="52"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="52"/>
+      <c r="B51" s="52"/>
+      <c r="C51" s="52"/>
+      <c r="D51" s="52"/>
+      <c r="E51" s="52"/>
+      <c r="F51" s="52"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="52"/>
+      <c r="B52" s="52"/>
+      <c r="C52" s="52"/>
+      <c r="D52" s="52"/>
+      <c r="E52" s="52"/>
+      <c r="F52" s="52"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="52"/>
+      <c r="B55" s="52"/>
+      <c r="C55" s="52"/>
+      <c r="D55" s="52"/>
+      <c r="E55" s="52"/>
+      <c r="F55" s="52"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="52"/>
+      <c r="B56" s="52"/>
+      <c r="C56" s="52"/>
+      <c r="D56" s="52"/>
+      <c r="E56" s="52"/>
+      <c r="F56" s="52"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" s="52"/>
+      <c r="B57" s="52"/>
+      <c r="C57" s="52"/>
+      <c r="D57" s="52"/>
+      <c r="E57" s="52"/>
+      <c r="F57" s="52"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" s="52"/>
+      <c r="B58" s="52"/>
+      <c r="C58" s="52"/>
+      <c r="D58" s="52"/>
+      <c r="E58" s="52"/>
+      <c r="F58" s="52"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" s="52"/>
+      <c r="B59" s="52"/>
+      <c r="C59" s="52"/>
+      <c r="D59" s="52"/>
+      <c r="E59" s="52"/>
+      <c r="F59" s="52"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" s="52"/>
+      <c r="B60" s="52"/>
+      <c r="C60" s="52"/>
+      <c r="D60" s="52"/>
+      <c r="E60" s="52"/>
+      <c r="F60" s="52"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="33">
+    <mergeCell ref="A55:B60"/>
+    <mergeCell ref="C55:D60"/>
+    <mergeCell ref="E55:F60"/>
+    <mergeCell ref="A39:B44"/>
+    <mergeCell ref="C39:D44"/>
+    <mergeCell ref="E39:F44"/>
+    <mergeCell ref="A47:B52"/>
+    <mergeCell ref="C47:D52"/>
+    <mergeCell ref="E47:F52"/>
+    <mergeCell ref="I15:J20"/>
+    <mergeCell ref="I23:J28"/>
+    <mergeCell ref="I31:J36"/>
+    <mergeCell ref="K15:L20"/>
+    <mergeCell ref="K23:L28"/>
+    <mergeCell ref="K31:L36"/>
+    <mergeCell ref="A31:B36"/>
+    <mergeCell ref="C31:D36"/>
+    <mergeCell ref="E31:F36"/>
+    <mergeCell ref="G15:H20"/>
+    <mergeCell ref="G23:H28"/>
+    <mergeCell ref="G31:H36"/>
+    <mergeCell ref="F1:G2"/>
+    <mergeCell ref="A15:B20"/>
+    <mergeCell ref="C15:D20"/>
+    <mergeCell ref="E15:F20"/>
+    <mergeCell ref="A23:B28"/>
+    <mergeCell ref="C23:D28"/>
+    <mergeCell ref="E23:F28"/>
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="A6:A8"/>
     <mergeCell ref="A9:A11"/>
     <mergeCell ref="B1:C2"/>
     <mergeCell ref="D1:E2"/>
-    <mergeCell ref="F1:G2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Battle-templates in Unity & Updates StatsSheet
Opponents, classes and weapon templates for test in Unity.
Few more stats in Excel sheet
</commit_message>
<xml_diff>
--- a/Game Design/Assets.xlsx
+++ b/Game Design/Assets.xlsx
@@ -2637,7 +2637,7 @@
   <dimension ref="A1:T44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
@@ -6653,23 +6653,7 @@
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="C31:D36"/>
-    <mergeCell ref="E31:F36"/>
-    <mergeCell ref="I23:J28"/>
-    <mergeCell ref="I31:J36"/>
-    <mergeCell ref="G39:H44"/>
-    <mergeCell ref="F1:G2"/>
-    <mergeCell ref="A15:B20"/>
-    <mergeCell ref="C15:D20"/>
-    <mergeCell ref="E15:F20"/>
-    <mergeCell ref="A23:B28"/>
-    <mergeCell ref="C23:D28"/>
-    <mergeCell ref="E23:F28"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="A9:A11"/>
-    <mergeCell ref="B1:C2"/>
-    <mergeCell ref="D1:E2"/>
+    <mergeCell ref="I15:J20"/>
     <mergeCell ref="A31:B36"/>
     <mergeCell ref="K15:L20"/>
     <mergeCell ref="K23:L28"/>
@@ -6686,7 +6670,23 @@
     <mergeCell ref="G15:H20"/>
     <mergeCell ref="G23:H28"/>
     <mergeCell ref="G31:H36"/>
-    <mergeCell ref="I15:J20"/>
+    <mergeCell ref="F1:G2"/>
+    <mergeCell ref="A15:B20"/>
+    <mergeCell ref="C15:D20"/>
+    <mergeCell ref="E15:F20"/>
+    <mergeCell ref="A23:B28"/>
+    <mergeCell ref="C23:D28"/>
+    <mergeCell ref="E23:F28"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="B1:C2"/>
+    <mergeCell ref="D1:E2"/>
+    <mergeCell ref="C31:D36"/>
+    <mergeCell ref="E31:F36"/>
+    <mergeCell ref="I23:J28"/>
+    <mergeCell ref="I31:J36"/>
+    <mergeCell ref="G39:H44"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>